<commit_message>
fix bug in simulaton module
</commit_message>
<xml_diff>
--- a/IO_M1_new/RunControl_M1_new.xlsx
+++ b/IO_M1_new/RunControl_M1_new.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7230" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
@@ -1372,10 +1372,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1384,13 +1381,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1497,16 +1497,16 @@
       <sheetName val="RunControl"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2039,17 +2039,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomRight" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="84.5703125" customWidth="1"/>
+    <col min="2" max="2" width="90" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
@@ -2236,61 +2236,61 @@
       </c>
     </row>
     <row r="4" spans="1:50" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="43"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="44" t="s">
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="44"/>
+      <c r="L4" s="43"/>
       <c r="M4" s="28"/>
-      <c r="N4" s="45" t="s">
+      <c r="N4" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="45"/>
-      <c r="P4" s="44" t="s">
+      <c r="O4" s="44"/>
+      <c r="P4" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
-      <c r="V4" s="44"/>
-      <c r="W4" s="44"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
       <c r="X4" s="29"/>
       <c r="Y4" s="29"/>
-      <c r="Z4" s="45" t="s">
+      <c r="Z4" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="AA4" s="45"/>
-      <c r="AB4" s="45"/>
-      <c r="AC4" s="47" t="s">
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="AD4" s="47"/>
-      <c r="AE4" s="47"/>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="42"/>
       <c r="AF4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AG4" s="42" t="s">
+      <c r="AG4" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="AH4" s="42"/>
-      <c r="AI4" s="42"/>
+      <c r="AH4" s="45"/>
+      <c r="AI4" s="45"/>
       <c r="AJ4" s="21" t="s">
         <v>70</v>
       </c>
@@ -2298,17 +2298,17 @@
       <c r="AL4" s="21"/>
       <c r="AM4" s="21"/>
       <c r="AN4" s="21"/>
-      <c r="AO4" s="47" t="s">
+      <c r="AO4" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="AP4" s="47"/>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="48" t="s">
+      <c r="AP4" s="42"/>
+      <c r="AQ4" s="42"/>
+      <c r="AR4" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="AS4" s="48"/>
-      <c r="AT4" s="48"/>
-      <c r="AU4" s="48"/>
+      <c r="AS4" s="46"/>
+      <c r="AT4" s="46"/>
+      <c r="AU4" s="46"/>
       <c r="AV4" s="15"/>
       <c r="AW4" s="22"/>
       <c r="AX4" s="20"/>
@@ -3195,7 +3195,7 @@
         <v>156</v>
       </c>
       <c r="AD14" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE14" s="26">
         <v>0.12</v>
@@ -3347,7 +3347,7 @@
         <v>156</v>
       </c>
       <c r="AD15" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE15" s="26">
         <v>0.12</v>
@@ -3499,7 +3499,7 @@
         <v>156</v>
       </c>
       <c r="AD16" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE16" s="26">
         <v>0.12</v>
@@ -3651,7 +3651,7 @@
         <v>156</v>
       </c>
       <c r="AD17" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE17" s="26">
         <v>0.12</v>
@@ -3803,7 +3803,7 @@
         <v>156</v>
       </c>
       <c r="AD18" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE18" s="26">
         <v>0.12</v>
@@ -3955,7 +3955,7 @@
         <v>156</v>
       </c>
       <c r="AD19" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE19" s="26">
         <v>0.12</v>
@@ -4107,7 +4107,7 @@
         <v>156</v>
       </c>
       <c r="AD20" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE20" s="26">
         <v>0.12</v>
@@ -4259,7 +4259,7 @@
         <v>156</v>
       </c>
       <c r="AD21" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE21" s="26">
         <v>0.12</v>
@@ -4411,7 +4411,7 @@
         <v>156</v>
       </c>
       <c r="AD22" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE22" s="26">
         <v>0.12</v>
@@ -4563,7 +4563,7 @@
         <v>156</v>
       </c>
       <c r="AD23" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE23" s="26">
         <v>0.12</v>
@@ -4715,7 +4715,7 @@
         <v>156</v>
       </c>
       <c r="AD24" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE24" s="26">
         <v>0.12</v>
@@ -4895,7 +4895,7 @@
         <v>156</v>
       </c>
       <c r="AD26" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE26" s="26">
         <v>0.12</v>
@@ -5047,7 +5047,7 @@
         <v>156</v>
       </c>
       <c r="AD27" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE27" s="26">
         <v>0.12</v>
@@ -5199,7 +5199,7 @@
         <v>156</v>
       </c>
       <c r="AD28" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE28" s="26">
         <v>0.12</v>
@@ -5351,7 +5351,7 @@
         <v>156</v>
       </c>
       <c r="AD29" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE29" s="26">
         <v>0.12</v>
@@ -5503,7 +5503,7 @@
         <v>156</v>
       </c>
       <c r="AD30" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE30" s="26">
         <v>0.12</v>
@@ -5655,7 +5655,7 @@
         <v>156</v>
       </c>
       <c r="AD31" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE31" s="26">
         <v>0.12</v>
@@ -5828,7 +5828,7 @@
         <v>0.01</v>
       </c>
       <c r="AB33" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AC33" s="26" t="s">
         <v>156</v>
@@ -5980,7 +5980,7 @@
         <v>0.01</v>
       </c>
       <c r="AB34" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AC34" s="26" t="s">
         <v>156</v>
@@ -6132,7 +6132,7 @@
         <v>0.01</v>
       </c>
       <c r="AB35" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC35" s="26" t="s">
         <v>156</v>
@@ -6284,7 +6284,7 @@
         <v>0.01</v>
       </c>
       <c r="AB36" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC36" s="26" t="s">
         <v>156</v>
@@ -6418,7 +6418,7 @@
         <v>275</v>
       </c>
       <c r="C39" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
         <v>211</v>
@@ -6499,7 +6499,7 @@
         <v>346</v>
       </c>
       <c r="AD39" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE39" s="26">
         <v>0.12</v>
@@ -6570,7 +6570,7 @@
         <v>277</v>
       </c>
       <c r="C40" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
         <v>211</v>
@@ -6651,7 +6651,7 @@
         <v>346</v>
       </c>
       <c r="AD40" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE40" s="26">
         <v>0.12</v>
@@ -6803,7 +6803,7 @@
         <v>346</v>
       </c>
       <c r="AD41" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE41" s="26">
         <v>0.12</v>
@@ -6874,7 +6874,7 @@
         <v>281</v>
       </c>
       <c r="C42" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
         <v>211</v>
@@ -6955,7 +6955,7 @@
         <v>346</v>
       </c>
       <c r="AD42" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE42" s="26">
         <v>0.12</v>
@@ -7026,7 +7026,7 @@
         <v>283</v>
       </c>
       <c r="C43" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" t="s">
         <v>211</v>
@@ -7107,7 +7107,7 @@
         <v>346</v>
       </c>
       <c r="AD43" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE43" s="26">
         <v>0.12</v>
@@ -7236,7 +7236,7 @@
         <v>286</v>
       </c>
       <c r="C46" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" t="s">
         <v>211</v>
@@ -7388,7 +7388,7 @@
         <v>289</v>
       </c>
       <c r="C47" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" t="s">
         <v>211</v>
@@ -7534,17 +7534,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="AO4:AQ4"/>
     <mergeCell ref="P4:W4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AG4:AI4"/>
     <mergeCell ref="AR4:AU4"/>
     <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <dataValidations count="21">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM9 AM13:AM47">
@@ -7677,13 +7677,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -7725,7 +7725,7 @@
         <v>0.12</v>
       </c>
       <c r="D5">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -7753,7 +7753,7 @@
         <v>0.12</v>
       </c>
       <c r="D7">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -7781,12 +7781,12 @@
         <v>0.12</v>
       </c>
       <c r="D9">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
-        <v>280</v>
+        <v>349</v>
       </c>
       <c r="B10" s="26">
         <v>-0.25</v>
@@ -7800,7 +7800,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
-        <v>280</v>
+        <v>349</v>
       </c>
       <c r="B11" s="26">
         <v>7.4999999999999997E-2</v>
@@ -7809,7 +7809,7 @@
         <v>0.12</v>
       </c>
       <c r="D11">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -7837,7 +7837,7 @@
         <v>0.12</v>
       </c>
       <c r="D13">
-        <v>79</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -7904,7 +7904,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7942,13 +7942,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>1000</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>20</v>
@@ -7973,7 +7973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix bug in inv returns
</commit_message>
<xml_diff>
--- a/IO_M1_new/RunControl_M1_new.xlsx
+++ b/IO_M1_new/RunControl_M1_new.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="352">
   <si>
     <t>Sheet #</t>
   </si>
@@ -1118,6 +1118,12 @@
   </si>
   <si>
     <t>A1F075_O30pA10_a</t>
+  </si>
+  <si>
+    <t>A1F075_C30pA10</t>
+  </si>
+  <si>
+    <t>75% initial Funding; Closed 30-year cp, 10-year smoothing</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1378,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1381,16 +1390,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2037,13 +2043,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX47"/>
+  <dimension ref="A1:AX48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C49" sqref="C49"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C40:C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,61 +2242,61 @@
       </c>
     </row>
     <row r="4" spans="1:50" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="47" t="s">
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="47"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
-      <c r="H4" s="48" t="s">
+      <c r="H4" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="43" t="s">
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="43"/>
+      <c r="L4" s="44"/>
       <c r="M4" s="28"/>
-      <c r="N4" s="44" t="s">
+      <c r="N4" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="44"/>
-      <c r="P4" s="43" t="s">
+      <c r="O4" s="45"/>
+      <c r="P4" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
       <c r="X4" s="29"/>
       <c r="Y4" s="29"/>
-      <c r="Z4" s="44" t="s">
+      <c r="Z4" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AA4" s="44"/>
-      <c r="AB4" s="44"/>
-      <c r="AC4" s="42" t="s">
+      <c r="AA4" s="45"/>
+      <c r="AB4" s="45"/>
+      <c r="AC4" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="AD4" s="42"/>
-      <c r="AE4" s="42"/>
+      <c r="AD4" s="47"/>
+      <c r="AE4" s="47"/>
       <c r="AF4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AG4" s="45" t="s">
+      <c r="AG4" s="42" t="s">
         <v>67</v>
       </c>
-      <c r="AH4" s="45"/>
-      <c r="AI4" s="45"/>
+      <c r="AH4" s="42"/>
+      <c r="AI4" s="42"/>
       <c r="AJ4" s="21" t="s">
         <v>70</v>
       </c>
@@ -2298,17 +2304,17 @@
       <c r="AL4" s="21"/>
       <c r="AM4" s="21"/>
       <c r="AN4" s="21"/>
-      <c r="AO4" s="42" t="s">
+      <c r="AO4" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="AP4" s="42"/>
-      <c r="AQ4" s="42"/>
-      <c r="AR4" s="46" t="s">
+      <c r="AP4" s="47"/>
+      <c r="AQ4" s="47"/>
+      <c r="AR4" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="AS4" s="46"/>
-      <c r="AT4" s="46"/>
-      <c r="AU4" s="46"/>
+      <c r="AS4" s="48"/>
+      <c r="AT4" s="48"/>
+      <c r="AU4" s="48"/>
       <c r="AV4" s="15"/>
       <c r="AW4" s="22"/>
       <c r="AX4" s="20"/>
@@ -5567,11 +5573,11 @@
       </c>
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>258</v>
+      <c r="A31" s="34" t="s">
+        <v>350</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>259</v>
+        <v>351</v>
       </c>
       <c r="C31" s="11" t="b">
         <v>0</v>
@@ -5664,7 +5670,7 @@
         <v>112</v>
       </c>
       <c r="AG31" s="2" t="s">
-        <v>158</v>
+        <v>347</v>
       </c>
       <c r="AH31" s="2" t="s">
         <v>348</v>
@@ -5676,7 +5682,7 @@
         <v>115</v>
       </c>
       <c r="AK31">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AL31">
         <v>200</v>
@@ -5691,7 +5697,7 @@
         <v>166</v>
       </c>
       <c r="AP31" s="17">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AQ31">
         <v>200</v>
@@ -5719,190 +5725,190 @@
       </c>
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C32" s="11"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="26"/>
-      <c r="U32" s="26"/>
-      <c r="X32" s="26"/>
-      <c r="Y32" s="26"/>
-      <c r="Z32" s="26"/>
-      <c r="AA32" s="26"/>
-      <c r="AB32" s="26"/>
-      <c r="AC32" s="26"/>
-      <c r="AD32" s="41"/>
-      <c r="AE32" s="26"/>
-      <c r="AG32" s="2"/>
-      <c r="AH32" s="2"/>
-      <c r="AM32" s="2"/>
-      <c r="AO32" s="2"/>
-      <c r="AP32" s="17"/>
-      <c r="AR32" s="2"/>
-      <c r="AS32" s="12"/>
-      <c r="AT32" s="12"/>
-      <c r="AU32" s="12"/>
-      <c r="AV32" s="18"/>
-      <c r="AW32" s="18"/>
-      <c r="AX32" s="18"/>
+      <c r="A32" t="s">
+        <v>258</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C32" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>211</v>
+      </c>
+      <c r="E32" t="s">
+        <v>188</v>
+      </c>
+      <c r="F32">
+        <v>1000</v>
+      </c>
+      <c r="G32">
+        <v>500</v>
+      </c>
+      <c r="H32" t="s">
+        <v>109</v>
+      </c>
+      <c r="I32" t="s">
+        <v>109</v>
+      </c>
+      <c r="J32" t="s">
+        <v>208</v>
+      </c>
+      <c r="K32" t="s">
+        <v>167</v>
+      </c>
+      <c r="L32" t="s">
+        <v>215</v>
+      </c>
+      <c r="M32" t="s">
+        <v>202</v>
+      </c>
+      <c r="N32" s="26">
+        <v>0</v>
+      </c>
+      <c r="O32" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P32" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q32">
+        <v>3</v>
+      </c>
+      <c r="R32">
+        <v>75</v>
+      </c>
+      <c r="S32">
+        <v>50</v>
+      </c>
+      <c r="T32">
+        <v>60</v>
+      </c>
+      <c r="U32" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>10</v>
+      </c>
+      <c r="X32" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y32" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z32" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA32" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB32" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC32" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD32" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE32" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG32" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH32" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI32">
+        <v>30</v>
+      </c>
+      <c r="AJ32" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK32">
+        <v>5</v>
+      </c>
+      <c r="AL32">
+        <v>200</v>
+      </c>
+      <c r="AM32" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN32">
+        <v>1</v>
+      </c>
+      <c r="AO32" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP32" s="17">
+        <v>1</v>
+      </c>
+      <c r="AQ32">
+        <v>200</v>
+      </c>
+      <c r="AR32" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS32" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT32" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU32" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV32" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW32" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX32" s="18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>260</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="C33" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" t="s">
-        <v>211</v>
-      </c>
-      <c r="E33" t="s">
-        <v>188</v>
-      </c>
-      <c r="F33">
-        <v>1000</v>
-      </c>
-      <c r="G33">
-        <v>500</v>
-      </c>
-      <c r="H33" t="s">
-        <v>109</v>
-      </c>
-      <c r="I33" t="s">
-        <v>109</v>
-      </c>
-      <c r="J33" t="s">
-        <v>208</v>
-      </c>
-      <c r="K33" t="s">
-        <v>167</v>
-      </c>
-      <c r="L33" t="s">
-        <v>215</v>
-      </c>
-      <c r="M33" t="s">
-        <v>202</v>
-      </c>
-      <c r="N33" s="26">
-        <v>0</v>
-      </c>
-      <c r="O33" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P33" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q33">
-        <v>3</v>
-      </c>
-      <c r="R33">
-        <v>75</v>
-      </c>
-      <c r="S33">
-        <v>50</v>
-      </c>
-      <c r="T33">
-        <v>60</v>
-      </c>
-      <c r="U33" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V33">
-        <v>0</v>
-      </c>
-      <c r="W33">
-        <v>10</v>
-      </c>
-      <c r="X33" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y33" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z33" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA33" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB33" s="26">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="AC33" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD33" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE33" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF33" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG33" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH33" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI33">
-        <v>15</v>
-      </c>
-      <c r="AJ33" t="s">
-        <v>115</v>
-      </c>
-      <c r="AK33">
-        <v>5</v>
-      </c>
-      <c r="AL33">
-        <v>200</v>
-      </c>
-      <c r="AM33" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN33">
-        <v>1</v>
-      </c>
-      <c r="AO33" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP33" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ33">
-        <v>200</v>
-      </c>
-      <c r="AR33" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS33" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT33" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU33" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV33" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW33" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX33" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="C33" s="11"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="26"/>
+      <c r="U33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="26"/>
+      <c r="AA33" s="26"/>
+      <c r="AB33" s="26"/>
+      <c r="AC33" s="26"/>
+      <c r="AD33" s="41"/>
+      <c r="AE33" s="26"/>
+      <c r="AG33" s="2"/>
+      <c r="AH33" s="2"/>
+      <c r="AM33" s="2"/>
+      <c r="AO33" s="2"/>
+      <c r="AP33" s="17"/>
+      <c r="AR33" s="2"/>
+      <c r="AS33" s="12"/>
+      <c r="AT33" s="12"/>
+      <c r="AU33" s="12"/>
+      <c r="AV33" s="18"/>
+      <c r="AW33" s="18"/>
+      <c r="AX33" s="18"/>
     </row>
     <row r="34" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>262</v>
+      <c r="A34" s="36" t="s">
+        <v>260</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C34" s="11" t="b">
         <v>0</v>
@@ -5986,7 +5992,7 @@
         <v>156</v>
       </c>
       <c r="AD34" s="41">
-        <v>7.1199999999999999E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE34" s="26">
         <v>0.12</v>
@@ -6050,11 +6056,11 @@
       </c>
     </row>
     <row r="35" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A35" s="37" t="s">
-        <v>266</v>
+      <c r="A35" t="s">
+        <v>262</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C35" s="11" t="b">
         <v>0</v>
@@ -6132,13 +6138,13 @@
         <v>0.01</v>
       </c>
       <c r="AB35" s="26">
-        <v>5.8999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AC35" s="26" t="s">
         <v>156</v>
       </c>
       <c r="AD35" s="41">
-        <v>8.2199999999999995E-2</v>
+        <v>7.1199999999999999E-2</v>
       </c>
       <c r="AE35" s="26">
         <v>0.12</v>
@@ -6202,11 +6208,11 @@
       </c>
     </row>
     <row r="36" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>269</v>
+      <c r="A36" s="37" t="s">
+        <v>266</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C36" s="11" t="b">
         <v>0</v>
@@ -6290,7 +6296,7 @@
         <v>156</v>
       </c>
       <c r="AD36" s="41">
-        <v>6.6199999999999995E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE36" s="26">
         <v>0.12</v>
@@ -6354,36 +6360,158 @@
       </c>
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C37" s="11"/>
-      <c r="N37" s="26"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="26"/>
-      <c r="U37" s="26"/>
-      <c r="X37" s="26"/>
-      <c r="Y37" s="26"/>
-      <c r="Z37" s="26"/>
-      <c r="AA37" s="26"/>
-      <c r="AB37" s="26"/>
-      <c r="AC37" s="26"/>
-      <c r="AD37" s="41"/>
-      <c r="AE37" s="26"/>
-      <c r="AG37" s="2"/>
-      <c r="AH37" s="2"/>
-      <c r="AM37" s="2"/>
-      <c r="AO37" s="2"/>
-      <c r="AP37" s="17"/>
-      <c r="AR37" s="2"/>
-      <c r="AS37" s="12"/>
-      <c r="AT37" s="12"/>
-      <c r="AU37" s="12"/>
-      <c r="AV37" s="18"/>
-      <c r="AW37" s="18"/>
-      <c r="AX37" s="18"/>
+      <c r="A37" t="s">
+        <v>269</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="C37" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" t="s">
+        <v>211</v>
+      </c>
+      <c r="E37" t="s">
+        <v>188</v>
+      </c>
+      <c r="F37">
+        <v>1000</v>
+      </c>
+      <c r="G37">
+        <v>500</v>
+      </c>
+      <c r="H37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I37" t="s">
+        <v>109</v>
+      </c>
+      <c r="J37" t="s">
+        <v>208</v>
+      </c>
+      <c r="K37" t="s">
+        <v>167</v>
+      </c>
+      <c r="L37" t="s">
+        <v>215</v>
+      </c>
+      <c r="M37" t="s">
+        <v>202</v>
+      </c>
+      <c r="N37" s="26">
+        <v>0</v>
+      </c>
+      <c r="O37" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P37" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q37">
+        <v>3</v>
+      </c>
+      <c r="R37">
+        <v>75</v>
+      </c>
+      <c r="S37">
+        <v>50</v>
+      </c>
+      <c r="T37">
+        <v>60</v>
+      </c>
+      <c r="U37" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>10</v>
+      </c>
+      <c r="X37" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y37" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z37" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA37" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB37" s="26">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AC37" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD37" s="41">
+        <v>6.6199999999999995E-2</v>
+      </c>
+      <c r="AE37" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG37" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH37" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI37">
+        <v>15</v>
+      </c>
+      <c r="AJ37" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK37">
+        <v>5</v>
+      </c>
+      <c r="AL37">
+        <v>200</v>
+      </c>
+      <c r="AM37" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN37">
+        <v>1</v>
+      </c>
+      <c r="AO37" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP37" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ37">
+        <v>200</v>
+      </c>
+      <c r="AR37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS37" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT37" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU37" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV37" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW37" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX37" s="18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B38" s="39" t="s">
-        <v>273</v>
-      </c>
       <c r="C38" s="11"/>
       <c r="N38" s="26"/>
       <c r="O38" s="18"/>
@@ -6411,163 +6539,41 @@
       <c r="AX38" s="18"/>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>274</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="C39" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D39" t="s">
-        <v>211</v>
-      </c>
-      <c r="E39" t="s">
-        <v>188</v>
-      </c>
-      <c r="F39">
-        <v>1000</v>
-      </c>
-      <c r="G39">
-        <v>500</v>
-      </c>
-      <c r="H39" t="s">
-        <v>109</v>
-      </c>
-      <c r="I39" t="s">
-        <v>109</v>
-      </c>
-      <c r="J39" t="s">
-        <v>208</v>
-      </c>
-      <c r="K39" t="s">
-        <v>167</v>
-      </c>
-      <c r="L39" t="s">
-        <v>215</v>
-      </c>
-      <c r="M39" t="s">
-        <v>202</v>
-      </c>
-      <c r="N39" s="26">
-        <v>0</v>
-      </c>
-      <c r="O39" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P39" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q39">
-        <v>3</v>
-      </c>
-      <c r="R39">
-        <v>75</v>
-      </c>
-      <c r="S39">
-        <v>50</v>
-      </c>
-      <c r="T39">
-        <v>60</v>
-      </c>
-      <c r="U39" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V39">
-        <v>0</v>
-      </c>
-      <c r="W39">
-        <v>10</v>
-      </c>
-      <c r="X39" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y39" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z39" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA39" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB39" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC39" s="26" t="s">
-        <v>346</v>
-      </c>
-      <c r="AD39" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE39" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF39" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG39" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH39" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AI39">
-        <v>1</v>
-      </c>
-      <c r="AJ39" t="s">
-        <v>142</v>
-      </c>
-      <c r="AK39">
-        <v>5</v>
-      </c>
-      <c r="AL39">
-        <v>200</v>
-      </c>
-      <c r="AM39" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN39">
-        <v>1</v>
-      </c>
-      <c r="AO39" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP39" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ39">
-        <v>200</v>
-      </c>
-      <c r="AR39" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS39" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT39" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU39" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV39" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW39" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX39" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="B39" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="X39" s="26"/>
+      <c r="Y39" s="26"/>
+      <c r="Z39" s="26"/>
+      <c r="AA39" s="26"/>
+      <c r="AB39" s="26"/>
+      <c r="AC39" s="26"/>
+      <c r="AD39" s="41"/>
+      <c r="AE39" s="26"/>
+      <c r="AG39" s="2"/>
+      <c r="AH39" s="2"/>
+      <c r="AM39" s="2"/>
+      <c r="AO39" s="2"/>
+      <c r="AP39" s="17"/>
+      <c r="AR39" s="2"/>
+      <c r="AS39" s="12"/>
+      <c r="AT39" s="12"/>
+      <c r="AU39" s="12"/>
+      <c r="AV39" s="18"/>
+      <c r="AW39" s="18"/>
+      <c r="AX39" s="18"/>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A40" s="34" t="s">
-        <v>276</v>
+      <c r="A40" t="s">
+        <v>274</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C40" s="11" t="b">
         <v>1</v>
@@ -6663,10 +6669,10 @@
         <v>158</v>
       </c>
       <c r="AH40" s="2" t="s">
-        <v>348</v>
+        <v>179</v>
       </c>
       <c r="AI40">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AJ40" t="s">
         <v>142</v>
@@ -6716,10 +6722,10 @@
     </row>
     <row r="41" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A41" s="34" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C41" s="11" t="b">
         <v>1</v>
@@ -6821,7 +6827,7 @@
         <v>30</v>
       </c>
       <c r="AJ41" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="AK41">
         <v>5</v>
@@ -6868,10 +6874,10 @@
     </row>
     <row r="42" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A42" s="34" t="s">
-        <v>349</v>
+        <v>278</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C42" s="11" t="b">
         <v>1</v>
@@ -6976,7 +6982,7 @@
         <v>115</v>
       </c>
       <c r="AK42">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AL42">
         <v>200</v>
@@ -7019,11 +7025,11 @@
       </c>
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A43" s="40" t="s">
-        <v>282</v>
+      <c r="A43" s="34" t="s">
+        <v>349</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C43" s="11" t="b">
         <v>1</v>
@@ -7128,7 +7134,7 @@
         <v>115</v>
       </c>
       <c r="AK43">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AL43">
         <v>200</v>
@@ -7143,7 +7149,7 @@
         <v>166</v>
       </c>
       <c r="AP43" s="17">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AQ43">
         <v>200</v>
@@ -7171,37 +7177,159 @@
       </c>
     </row>
     <row r="44" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
-      <c r="C44" s="11"/>
-      <c r="N44" s="26"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="26"/>
-      <c r="U44" s="26"/>
-      <c r="X44" s="26"/>
-      <c r="Y44" s="26"/>
-      <c r="Z44" s="26"/>
-      <c r="AA44" s="26"/>
-      <c r="AB44" s="26"/>
-      <c r="AC44" s="26"/>
-      <c r="AD44" s="41"/>
-      <c r="AE44" s="26"/>
-      <c r="AG44" s="2"/>
-      <c r="AH44" s="2"/>
-      <c r="AM44" s="2"/>
-      <c r="AO44" s="2"/>
-      <c r="AP44" s="17"/>
-      <c r="AR44" s="2"/>
-      <c r="AS44" s="12"/>
-      <c r="AT44" s="12"/>
-      <c r="AU44" s="12"/>
-      <c r="AV44" s="18"/>
-      <c r="AW44" s="18"/>
-      <c r="AX44" s="18"/>
+      <c r="A44" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="C44" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>211</v>
+      </c>
+      <c r="E44" t="s">
+        <v>188</v>
+      </c>
+      <c r="F44">
+        <v>1000</v>
+      </c>
+      <c r="G44">
+        <v>500</v>
+      </c>
+      <c r="H44" t="s">
+        <v>109</v>
+      </c>
+      <c r="I44" t="s">
+        <v>109</v>
+      </c>
+      <c r="J44" t="s">
+        <v>208</v>
+      </c>
+      <c r="K44" t="s">
+        <v>167</v>
+      </c>
+      <c r="L44" t="s">
+        <v>215</v>
+      </c>
+      <c r="M44" t="s">
+        <v>202</v>
+      </c>
+      <c r="N44" s="26">
+        <v>0</v>
+      </c>
+      <c r="O44" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P44" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q44">
+        <v>3</v>
+      </c>
+      <c r="R44">
+        <v>75</v>
+      </c>
+      <c r="S44">
+        <v>50</v>
+      </c>
+      <c r="T44">
+        <v>60</v>
+      </c>
+      <c r="U44" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44">
+        <v>10</v>
+      </c>
+      <c r="X44" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y44" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z44" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA44" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB44" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC44" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD44" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE44" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF44" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG44" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH44" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI44">
+        <v>30</v>
+      </c>
+      <c r="AJ44" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK44">
+        <v>5</v>
+      </c>
+      <c r="AL44">
+        <v>200</v>
+      </c>
+      <c r="AM44" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN44">
+        <v>1</v>
+      </c>
+      <c r="AO44" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP44" s="17">
+        <v>1</v>
+      </c>
+      <c r="AQ44">
+        <v>200</v>
+      </c>
+      <c r="AR44" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS44" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT44" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU44" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV44" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW44" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX44" s="18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B45" s="31" t="s">
-        <v>284</v>
-      </c>
+      <c r="A45" s="40"/>
       <c r="C45" s="11"/>
       <c r="N45" s="26"/>
       <c r="O45" s="18"/>
@@ -7229,166 +7357,44 @@
       <c r="AX45" s="18"/>
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A46" s="34" t="s">
-        <v>285</v>
-      </c>
-      <c r="B46" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="C46" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" t="s">
-        <v>211</v>
-      </c>
-      <c r="E46" t="s">
-        <v>188</v>
-      </c>
-      <c r="F46">
-        <v>1000</v>
-      </c>
-      <c r="G46">
-        <v>500</v>
-      </c>
-      <c r="H46" t="s">
-        <v>109</v>
-      </c>
-      <c r="I46" t="s">
-        <v>109</v>
-      </c>
-      <c r="J46" t="s">
-        <v>208</v>
-      </c>
-      <c r="K46" t="s">
-        <v>167</v>
-      </c>
-      <c r="L46" t="s">
-        <v>215</v>
-      </c>
-      <c r="M46" t="s">
-        <v>202</v>
-      </c>
-      <c r="N46" s="26">
-        <v>0</v>
-      </c>
-      <c r="O46" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P46" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q46">
-        <v>3</v>
-      </c>
-      <c r="R46">
-        <v>75</v>
-      </c>
-      <c r="S46">
-        <v>50</v>
-      </c>
-      <c r="T46">
-        <v>60</v>
-      </c>
-      <c r="U46" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V46">
-        <v>0</v>
-      </c>
-      <c r="W46">
-        <v>10</v>
-      </c>
-      <c r="X46" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y46" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z46" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA46" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB46" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC46" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD46" s="41">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AE46" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF46" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG46" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH46" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI46">
-        <v>30</v>
-      </c>
-      <c r="AJ46" t="s">
-        <v>115</v>
-      </c>
-      <c r="AK46">
-        <v>5</v>
-      </c>
-      <c r="AL46">
-        <v>200</v>
-      </c>
-      <c r="AM46" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN46">
-        <v>1</v>
-      </c>
-      <c r="AO46" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP46" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ46">
-        <v>200</v>
-      </c>
-      <c r="AR46" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS46" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT46" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU46" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV46" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW46" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX46" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="B46" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="C46" s="11"/>
+      <c r="N46" s="26"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="26"/>
+      <c r="U46" s="26"/>
+      <c r="X46" s="26"/>
+      <c r="Y46" s="26"/>
+      <c r="Z46" s="26"/>
+      <c r="AA46" s="26"/>
+      <c r="AB46" s="26"/>
+      <c r="AC46" s="26"/>
+      <c r="AD46" s="41"/>
+      <c r="AE46" s="26"/>
+      <c r="AG46" s="2"/>
+      <c r="AH46" s="2"/>
+      <c r="AM46" s="2"/>
+      <c r="AO46" s="2"/>
+      <c r="AP46" s="17"/>
+      <c r="AR46" s="2"/>
+      <c r="AS46" s="12"/>
+      <c r="AT46" s="12"/>
+      <c r="AU46" s="12"/>
+      <c r="AV46" s="18"/>
+      <c r="AW46" s="18"/>
+      <c r="AX46" s="18"/>
     </row>
     <row r="47" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A47" s="34" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C47" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
         <v>211</v>
@@ -7469,7 +7475,7 @@
         <v>156</v>
       </c>
       <c r="AD47" s="41">
-        <v>8.2199999999999995E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="AE47" s="26">
         <v>0.12</v>
@@ -7529,100 +7535,252 @@
         <v>1</v>
       </c>
       <c r="AX47" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A48" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="C48" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" t="s">
+        <v>211</v>
+      </c>
+      <c r="E48" t="s">
+        <v>188</v>
+      </c>
+      <c r="F48">
+        <v>1000</v>
+      </c>
+      <c r="G48">
+        <v>500</v>
+      </c>
+      <c r="H48" t="s">
+        <v>109</v>
+      </c>
+      <c r="I48" t="s">
+        <v>109</v>
+      </c>
+      <c r="J48" t="s">
+        <v>208</v>
+      </c>
+      <c r="K48" t="s">
+        <v>167</v>
+      </c>
+      <c r="L48" t="s">
+        <v>215</v>
+      </c>
+      <c r="M48" t="s">
+        <v>202</v>
+      </c>
+      <c r="N48" s="26">
+        <v>0</v>
+      </c>
+      <c r="O48" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P48" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q48">
+        <v>3</v>
+      </c>
+      <c r="R48">
+        <v>75</v>
+      </c>
+      <c r="S48">
+        <v>50</v>
+      </c>
+      <c r="T48">
+        <v>60</v>
+      </c>
+      <c r="U48" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V48">
+        <v>0</v>
+      </c>
+      <c r="W48">
+        <v>10</v>
+      </c>
+      <c r="X48" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y48" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z48" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA48" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB48" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC48" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD48" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE48" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF48" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG48" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH48" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI48">
+        <v>30</v>
+      </c>
+      <c r="AJ48" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK48">
+        <v>5</v>
+      </c>
+      <c r="AL48">
+        <v>200</v>
+      </c>
+      <c r="AM48" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN48">
+        <v>1</v>
+      </c>
+      <c r="AO48" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP48" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ48">
+        <v>200</v>
+      </c>
+      <c r="AR48" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS48" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT48" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU48" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV48" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW48" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX48" s="18" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="H4:J4"/>
     <mergeCell ref="AO4:AQ4"/>
     <mergeCell ref="P4:W4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AG4:AI4"/>
     <mergeCell ref="AR4:AU4"/>
     <mergeCell ref="AC4:AE4"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <dataValidations count="21">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM9 AM13:AM47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM9 AM13:AM48">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH9 AH13:AH47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH9 AH13:AH48">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AG9 AG13:AG47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AG9 AG13:AG48">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR6:AR9 AR13:AR47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR6:AR9 AR13:AR48">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O9 C6:C10 O13:O47 C13:C47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O9 C6:C10 O13:O48 C13:C48">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="AA6:AA9 U6:U9 AA13:AA47 U13:U47">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="AA6:AA9 U6:U9 U13:U48 AA13:AA48">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="V6:W9 V13:W47">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="V6:W9 V13:W48">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Z9 AB6:AB9 AD6:AD9 X13:Z47 AB13:AB47 AD13:AD47">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Z9 AB6:AB9 AD6:AD9 AD13:AD48 AB13:AB48 X13:Z48">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AI6:AI9 AI13:AI47">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AI6:AI9 AI13:AI48">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AS6:AT9 AS13:AT47">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AS6:AT9 AS13:AT48">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AU6:AU9 AU13:AU47">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AU6:AU9 AU13:AU48">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AE6:AE9 AE13:AE47">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AE6:AE9 AE13:AE48">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AK6:AK9 AK13:AK47">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AK6:AK9 AK13:AK48">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL9 AL13:AL47">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL9 AL13:AL48">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN13:AN47">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN13:AN48">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AC6:AC9 AC13:AC47"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV6:AX9 AV13:AX47">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AC6:AC9 AC13:AC48"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV6:AX9 AV13:AX48">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO9 AO13:AO47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO9 AO13:AO48">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP9 AP13:AP47">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP9 AP13:AP48">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="R6:R9 R13:R47">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="R6:R9 R13:R48">
       <formula1>35</formula1>
       <formula2>80</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:I9 H13:I47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:I9 H13:I48">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -7635,37 +7793,37 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$57:$A$61</xm:f>
           </x14:formula1>
-          <xm:sqref>K6:K9 K13:K47</xm:sqref>
+          <xm:sqref>K6:K9 K13:K48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$64:$A$71</xm:f>
           </x14:formula1>
-          <xm:sqref>L6:L9 L13:L47</xm:sqref>
+          <xm:sqref>L6:L9 L13:L48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$45:$A$52</xm:f>
           </x14:formula1>
-          <xm:sqref>E6:E9 E13:E47</xm:sqref>
+          <xm:sqref>E6:E9 E13:E48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$29:$A$42</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:D9 D13:D47</xm:sqref>
+          <xm:sqref>D6:D9 D13:D48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$21:$A$24</xm:f>
           </x14:formula1>
-          <xm:sqref>J6:J9 J13:J47</xm:sqref>
+          <xm:sqref>J6:J9 J13:J48</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$74:$A$77</xm:f>
           </x14:formula1>
-          <xm:sqref>M6:M9 M13:M47</xm:sqref>
+          <xm:sqref>M6:M9 M13:M48</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7678,7 +7836,7 @@
   <dimension ref="A3:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7719,7 +7877,7 @@
         <v>274</v>
       </c>
       <c r="B5" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="C5" s="26">
         <v>0.12</v>
@@ -7747,7 +7905,7 @@
         <v>276</v>
       </c>
       <c r="B7" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="C7" s="26">
         <v>0.12</v>
@@ -7775,7 +7933,7 @@
         <v>278</v>
       </c>
       <c r="B9" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="C9" s="26">
         <v>0.12</v>
@@ -7803,7 +7961,7 @@
         <v>349</v>
       </c>
       <c r="B11" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="C11" s="26">
         <v>0.12</v>
@@ -7831,7 +7989,7 @@
         <v>282</v>
       </c>
       <c r="B13" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="C13" s="26">
         <v>0.12</v>

</xml_diff>

<commit_message>
small improvements on functions and runs
</commit_message>
<xml_diff>
--- a/IO_M1_new/RunControl_M1_new.xlsx
+++ b/IO_M1_new/RunControl_M1_new.xlsx
@@ -2046,16 +2046,16 @@
   <dimension ref="A1:AX48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C40" sqref="C40:C44"/>
+      <selection pane="bottomRight" activeCell="C34" sqref="C34:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
-    <col min="2" max="2" width="90" customWidth="1"/>
+    <col min="2" max="2" width="98.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
@@ -5911,7 +5911,7 @@
         <v>261</v>
       </c>
       <c r="C34" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
         <v>211</v>
@@ -6025,13 +6025,14 @@
         <v>1</v>
       </c>
       <c r="AO34" s="2" t="s">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="AP34" s="17">
         <v>0.75</v>
       </c>
-      <c r="AQ34">
-        <v>200</v>
+      <c r="AQ34" s="25">
+        <f>225068282*0.75</f>
+        <v>168801211.5</v>
       </c>
       <c r="AR34" s="2" t="s">
         <v>113</v>
@@ -6063,7 +6064,7 @@
         <v>263</v>
       </c>
       <c r="C35" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" t="s">
         <v>211</v>
@@ -6177,13 +6178,14 @@
         <v>1</v>
       </c>
       <c r="AO35" s="2" t="s">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="AP35" s="17">
         <v>0.75</v>
       </c>
-      <c r="AQ35">
-        <v>200</v>
+      <c r="AQ35" s="25">
+        <f t="shared" ref="AQ35:AQ37" si="0">225068282*0.75</f>
+        <v>168801211.5</v>
       </c>
       <c r="AR35" s="2" t="s">
         <v>113</v>
@@ -6215,7 +6217,7 @@
         <v>267</v>
       </c>
       <c r="C36" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>211</v>
@@ -6329,13 +6331,14 @@
         <v>1</v>
       </c>
       <c r="AO36" s="2" t="s">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="AP36" s="17">
         <v>0.75</v>
       </c>
-      <c r="AQ36">
-        <v>200</v>
+      <c r="AQ36" s="25">
+        <f t="shared" si="0"/>
+        <v>168801211.5</v>
       </c>
       <c r="AR36" s="2" t="s">
         <v>113</v>
@@ -6367,7 +6370,7 @@
         <v>270</v>
       </c>
       <c r="C37" s="11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
         <v>211</v>
@@ -6481,13 +6484,14 @@
         <v>1</v>
       </c>
       <c r="AO37" s="2" t="s">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="AP37" s="17">
         <v>0.75</v>
       </c>
-      <c r="AQ37">
-        <v>200</v>
+      <c r="AQ37" s="25">
+        <f t="shared" si="0"/>
+        <v>168801211.5</v>
       </c>
       <c r="AR37" s="2" t="s">
         <v>113</v>
@@ -6576,7 +6580,7 @@
         <v>275</v>
       </c>
       <c r="C40" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" t="s">
         <v>211</v>
@@ -6728,7 +6732,7 @@
         <v>277</v>
       </c>
       <c r="C41" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41" t="s">
         <v>211</v>
@@ -6880,7 +6884,7 @@
         <v>279</v>
       </c>
       <c r="C42" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D42" t="s">
         <v>211</v>
@@ -7032,7 +7036,7 @@
         <v>281</v>
       </c>
       <c r="C43" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" t="s">
         <v>211</v>
@@ -7184,7 +7188,7 @@
         <v>283</v>
       </c>
       <c r="C44" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" t="s">
         <v>211</v>

</xml_diff>

<commit_message>
changes in result anaylsis
</commit_message>
<xml_diff>
--- a/IO_M1_new/RunControl_M1_new.xlsx
+++ b/IO_M1_new/RunControl_M1_new.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="353">
   <si>
     <t>Sheet #</t>
   </si>
@@ -1124,6 +1124,9 @@
   </si>
   <si>
     <t>75% initial Funding; Closed 30-year cp, 10-year smoothing</t>
+  </si>
+  <si>
+    <t>A1F100_O30pA5_cap</t>
   </si>
 </sst>
 </file>
@@ -2043,18 +2046,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX48"/>
+  <dimension ref="A1:AX52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="AL22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C34" sqref="C34:C37"/>
+      <selection pane="bottomRight" activeCell="AR39" sqref="AR39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
     <col min="2" max="2" width="98.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
@@ -6494,7 +6497,7 @@
         <v>168801211.5</v>
       </c>
       <c r="AR37" s="2" t="s">
-        <v>113</v>
+        <v>134</v>
       </c>
       <c r="AS37" s="12">
         <v>0.25</v>
@@ -6516,6 +6519,7 @@
       </c>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B38" s="19"/>
       <c r="C38" s="11"/>
       <c r="N38" s="26"/>
       <c r="O38" s="18"/>
@@ -6534,6 +6538,7 @@
       <c r="AM38" s="2"/>
       <c r="AO38" s="2"/>
       <c r="AP38" s="17"/>
+      <c r="AQ38" s="25"/>
       <c r="AR38" s="2"/>
       <c r="AS38" s="12"/>
       <c r="AT38" s="12"/>
@@ -6543,649 +6548,277 @@
       <c r="AX38" s="18"/>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B39" s="39" t="s">
-        <v>273</v>
-      </c>
-      <c r="C39" s="11"/>
-      <c r="N39" s="26"/>
-      <c r="O39" s="18"/>
-      <c r="P39" s="26"/>
-      <c r="U39" s="26"/>
-      <c r="X39" s="26"/>
-      <c r="Y39" s="26"/>
-      <c r="Z39" s="26"/>
-      <c r="AA39" s="26"/>
-      <c r="AB39" s="26"/>
-      <c r="AC39" s="26"/>
-      <c r="AD39" s="41"/>
-      <c r="AE39" s="26"/>
-      <c r="AG39" s="2"/>
-      <c r="AH39" s="2"/>
-      <c r="AM39" s="2"/>
-      <c r="AO39" s="2"/>
-      <c r="AP39" s="17"/>
-      <c r="AR39" s="2"/>
-      <c r="AS39" s="12"/>
-      <c r="AT39" s="12"/>
-      <c r="AU39" s="12"/>
-      <c r="AV39" s="18"/>
-      <c r="AW39" s="18"/>
-      <c r="AX39" s="18"/>
+      <c r="A39" t="s">
+        <v>352</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C39" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E39" t="s">
+        <v>188</v>
+      </c>
+      <c r="F39">
+        <v>1000</v>
+      </c>
+      <c r="G39">
+        <v>500</v>
+      </c>
+      <c r="H39" t="s">
+        <v>109</v>
+      </c>
+      <c r="I39" t="s">
+        <v>109</v>
+      </c>
+      <c r="J39" t="s">
+        <v>208</v>
+      </c>
+      <c r="K39" t="s">
+        <v>167</v>
+      </c>
+      <c r="L39" t="s">
+        <v>215</v>
+      </c>
+      <c r="M39" t="s">
+        <v>202</v>
+      </c>
+      <c r="N39" s="26">
+        <v>0</v>
+      </c>
+      <c r="O39" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P39" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q39">
+        <v>3</v>
+      </c>
+      <c r="R39">
+        <v>75</v>
+      </c>
+      <c r="S39">
+        <v>50</v>
+      </c>
+      <c r="T39">
+        <v>60</v>
+      </c>
+      <c r="U39" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>10</v>
+      </c>
+      <c r="X39" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y39" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z39" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA39" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB39" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC39" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD39" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE39" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF39" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG39" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH39" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI39">
+        <v>30</v>
+      </c>
+      <c r="AJ39" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK39">
+        <v>5</v>
+      </c>
+      <c r="AL39">
+        <v>200</v>
+      </c>
+      <c r="AM39" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN39">
+        <v>1</v>
+      </c>
+      <c r="AO39" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP39" s="17">
+        <v>1</v>
+      </c>
+      <c r="AQ39">
+        <v>200</v>
+      </c>
+      <c r="AR39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS39" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT39" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU39" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV39" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW39" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX39" s="18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>274</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="C40" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" t="s">
-        <v>211</v>
-      </c>
-      <c r="E40" t="s">
-        <v>188</v>
-      </c>
-      <c r="F40">
-        <v>1000</v>
-      </c>
-      <c r="G40">
-        <v>500</v>
-      </c>
-      <c r="H40" t="s">
-        <v>109</v>
-      </c>
-      <c r="I40" t="s">
-        <v>109</v>
-      </c>
-      <c r="J40" t="s">
-        <v>208</v>
-      </c>
-      <c r="K40" t="s">
-        <v>167</v>
-      </c>
-      <c r="L40" t="s">
-        <v>215</v>
-      </c>
-      <c r="M40" t="s">
-        <v>202</v>
-      </c>
-      <c r="N40" s="26">
-        <v>0</v>
-      </c>
-      <c r="O40" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P40" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q40">
-        <v>3</v>
-      </c>
-      <c r="R40">
-        <v>75</v>
-      </c>
-      <c r="S40">
-        <v>50</v>
-      </c>
-      <c r="T40">
-        <v>60</v>
-      </c>
-      <c r="U40" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V40">
-        <v>0</v>
-      </c>
-      <c r="W40">
-        <v>10</v>
-      </c>
-      <c r="X40" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y40" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z40" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA40" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB40" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC40" s="26" t="s">
-        <v>346</v>
-      </c>
-      <c r="AD40" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE40" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF40" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG40" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH40" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AI40">
-        <v>1</v>
-      </c>
-      <c r="AJ40" t="s">
-        <v>142</v>
-      </c>
-      <c r="AK40">
-        <v>5</v>
-      </c>
-      <c r="AL40">
-        <v>200</v>
-      </c>
-      <c r="AM40" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN40">
-        <v>1</v>
-      </c>
-      <c r="AO40" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP40" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ40">
-        <v>200</v>
-      </c>
-      <c r="AR40" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS40" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT40" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU40" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV40" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW40" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX40" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="B40" s="19"/>
+      <c r="C40" s="11"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="26"/>
+      <c r="U40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="26"/>
+      <c r="Z40" s="26"/>
+      <c r="AA40" s="26"/>
+      <c r="AB40" s="26"/>
+      <c r="AC40" s="26"/>
+      <c r="AD40" s="41"/>
+      <c r="AE40" s="26"/>
+      <c r="AG40" s="2"/>
+      <c r="AH40" s="2"/>
+      <c r="AM40" s="2"/>
+      <c r="AO40" s="2"/>
+      <c r="AP40" s="17"/>
+      <c r="AR40" s="2"/>
+      <c r="AS40" s="12"/>
+      <c r="AT40" s="12"/>
+      <c r="AU40" s="12"/>
+      <c r="AV40" s="18"/>
+      <c r="AW40" s="18"/>
+      <c r="AX40" s="18"/>
     </row>
     <row r="41" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="C41" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D41" t="s">
-        <v>211</v>
-      </c>
-      <c r="E41" t="s">
-        <v>188</v>
-      </c>
-      <c r="F41">
-        <v>1000</v>
-      </c>
-      <c r="G41">
-        <v>500</v>
-      </c>
-      <c r="H41" t="s">
-        <v>109</v>
-      </c>
-      <c r="I41" t="s">
-        <v>109</v>
-      </c>
-      <c r="J41" t="s">
-        <v>208</v>
-      </c>
-      <c r="K41" t="s">
-        <v>167</v>
-      </c>
-      <c r="L41" t="s">
-        <v>215</v>
-      </c>
-      <c r="M41" t="s">
-        <v>202</v>
-      </c>
-      <c r="N41" s="26">
-        <v>0</v>
-      </c>
-      <c r="O41" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P41" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q41">
-        <v>3</v>
-      </c>
-      <c r="R41">
-        <v>75</v>
-      </c>
-      <c r="S41">
-        <v>50</v>
-      </c>
-      <c r="T41">
-        <v>60</v>
-      </c>
-      <c r="U41" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V41">
-        <v>0</v>
-      </c>
-      <c r="W41">
-        <v>10</v>
-      </c>
-      <c r="X41" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y41" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z41" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA41" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB41" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC41" s="26" t="s">
-        <v>346</v>
-      </c>
-      <c r="AD41" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE41" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF41" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG41" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH41" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI41">
-        <v>30</v>
-      </c>
-      <c r="AJ41" t="s">
-        <v>142</v>
-      </c>
-      <c r="AK41">
-        <v>5</v>
-      </c>
-      <c r="AL41">
-        <v>200</v>
-      </c>
-      <c r="AM41" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN41">
-        <v>1</v>
-      </c>
-      <c r="AO41" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP41" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ41">
-        <v>200</v>
-      </c>
-      <c r="AR41" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS41" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT41" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU41" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV41" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW41" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX41" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="B41" s="19"/>
+      <c r="C41" s="11"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="26"/>
+      <c r="U41" s="26"/>
+      <c r="X41" s="26"/>
+      <c r="Y41" s="26"/>
+      <c r="Z41" s="26"/>
+      <c r="AA41" s="26"/>
+      <c r="AB41" s="26"/>
+      <c r="AC41" s="26"/>
+      <c r="AD41" s="41"/>
+      <c r="AE41" s="26"/>
+      <c r="AG41" s="2"/>
+      <c r="AH41" s="2"/>
+      <c r="AM41" s="2"/>
+      <c r="AO41" s="2"/>
+      <c r="AP41" s="17"/>
+      <c r="AQ41" s="25"/>
+      <c r="AR41" s="2"/>
+      <c r="AS41" s="12"/>
+      <c r="AT41" s="12"/>
+      <c r="AU41" s="12"/>
+      <c r="AV41" s="18"/>
+      <c r="AW41" s="18"/>
+      <c r="AX41" s="18"/>
     </row>
     <row r="42" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>278</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="C42" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D42" t="s">
-        <v>211</v>
-      </c>
-      <c r="E42" t="s">
-        <v>188</v>
-      </c>
-      <c r="F42">
-        <v>1000</v>
-      </c>
-      <c r="G42">
-        <v>500</v>
-      </c>
-      <c r="H42" t="s">
-        <v>109</v>
-      </c>
-      <c r="I42" t="s">
-        <v>109</v>
-      </c>
-      <c r="J42" t="s">
-        <v>208</v>
-      </c>
-      <c r="K42" t="s">
-        <v>167</v>
-      </c>
-      <c r="L42" t="s">
-        <v>215</v>
-      </c>
-      <c r="M42" t="s">
-        <v>202</v>
-      </c>
-      <c r="N42" s="26">
-        <v>0</v>
-      </c>
-      <c r="O42" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P42" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q42">
-        <v>3</v>
-      </c>
-      <c r="R42">
-        <v>75</v>
-      </c>
-      <c r="S42">
-        <v>50</v>
-      </c>
-      <c r="T42">
-        <v>60</v>
-      </c>
-      <c r="U42" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V42">
-        <v>0</v>
-      </c>
-      <c r="W42">
-        <v>10</v>
-      </c>
-      <c r="X42" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y42" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z42" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA42" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB42" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC42" s="26" t="s">
-        <v>346</v>
-      </c>
-      <c r="AD42" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE42" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF42" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG42" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH42" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI42">
-        <v>30</v>
-      </c>
-      <c r="AJ42" t="s">
-        <v>115</v>
-      </c>
-      <c r="AK42">
-        <v>5</v>
-      </c>
-      <c r="AL42">
-        <v>200</v>
-      </c>
-      <c r="AM42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN42">
-        <v>1</v>
-      </c>
-      <c r="AO42" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP42" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ42">
-        <v>200</v>
-      </c>
-      <c r="AR42" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS42" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT42" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU42" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV42" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW42" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX42" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="C42" s="11"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="26"/>
+      <c r="U42" s="26"/>
+      <c r="X42" s="26"/>
+      <c r="Y42" s="26"/>
+      <c r="Z42" s="26"/>
+      <c r="AA42" s="26"/>
+      <c r="AB42" s="26"/>
+      <c r="AC42" s="26"/>
+      <c r="AD42" s="41"/>
+      <c r="AE42" s="26"/>
+      <c r="AG42" s="2"/>
+      <c r="AH42" s="2"/>
+      <c r="AM42" s="2"/>
+      <c r="AO42" s="2"/>
+      <c r="AP42" s="17"/>
+      <c r="AR42" s="2"/>
+      <c r="AS42" s="12"/>
+      <c r="AT42" s="12"/>
+      <c r="AU42" s="12"/>
+      <c r="AV42" s="18"/>
+      <c r="AW42" s="18"/>
+      <c r="AX42" s="18"/>
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A43" s="34" t="s">
-        <v>349</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="C43" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="D43" t="s">
-        <v>211</v>
-      </c>
-      <c r="E43" t="s">
-        <v>188</v>
-      </c>
-      <c r="F43">
-        <v>1000</v>
-      </c>
-      <c r="G43">
-        <v>500</v>
-      </c>
-      <c r="H43" t="s">
-        <v>109</v>
-      </c>
-      <c r="I43" t="s">
-        <v>109</v>
-      </c>
-      <c r="J43" t="s">
-        <v>208</v>
-      </c>
-      <c r="K43" t="s">
-        <v>167</v>
-      </c>
-      <c r="L43" t="s">
-        <v>215</v>
-      </c>
-      <c r="M43" t="s">
-        <v>202</v>
-      </c>
-      <c r="N43" s="26">
-        <v>0</v>
-      </c>
-      <c r="O43" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P43" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q43">
-        <v>3</v>
-      </c>
-      <c r="R43">
-        <v>75</v>
-      </c>
-      <c r="S43">
-        <v>50</v>
-      </c>
-      <c r="T43">
-        <v>60</v>
-      </c>
-      <c r="U43" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V43">
-        <v>0</v>
-      </c>
-      <c r="W43">
-        <v>10</v>
-      </c>
-      <c r="X43" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y43" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z43" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA43" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB43" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC43" s="26" t="s">
-        <v>346</v>
-      </c>
-      <c r="AD43" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE43" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF43" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG43" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH43" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI43">
-        <v>30</v>
-      </c>
-      <c r="AJ43" t="s">
-        <v>115</v>
-      </c>
-      <c r="AK43">
-        <v>10</v>
-      </c>
-      <c r="AL43">
-        <v>200</v>
-      </c>
-      <c r="AM43" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN43">
-        <v>1</v>
-      </c>
-      <c r="AO43" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP43" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ43">
-        <v>200</v>
-      </c>
-      <c r="AR43" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS43" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT43" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU43" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV43" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW43" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX43" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="B43" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="26"/>
+      <c r="U43" s="26"/>
+      <c r="X43" s="26"/>
+      <c r="Y43" s="26"/>
+      <c r="Z43" s="26"/>
+      <c r="AA43" s="26"/>
+      <c r="AB43" s="26"/>
+      <c r="AC43" s="26"/>
+      <c r="AD43" s="41"/>
+      <c r="AE43" s="26"/>
+      <c r="AG43" s="2"/>
+      <c r="AH43" s="2"/>
+      <c r="AM43" s="2"/>
+      <c r="AO43" s="2"/>
+      <c r="AP43" s="17"/>
+      <c r="AR43" s="2"/>
+      <c r="AS43" s="12"/>
+      <c r="AT43" s="12"/>
+      <c r="AU43" s="12"/>
+      <c r="AV43" s="18"/>
+      <c r="AW43" s="18"/>
+      <c r="AX43" s="18"/>
     </row>
     <row r="44" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A44" s="40" t="s">
-        <v>282</v>
+      <c r="A44" t="s">
+        <v>274</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C44" s="11" t="b">
         <v>0</v>
@@ -7281,13 +6914,13 @@
         <v>158</v>
       </c>
       <c r="AH44" s="2" t="s">
-        <v>348</v>
+        <v>179</v>
       </c>
       <c r="AI44">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AJ44" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="AK44">
         <v>5</v>
@@ -7305,7 +6938,7 @@
         <v>166</v>
       </c>
       <c r="AP44" s="17">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AQ44">
         <v>200</v>
@@ -7333,69 +6966,315 @@
       </c>
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A45" s="40"/>
-      <c r="C45" s="11"/>
-      <c r="N45" s="26"/>
-      <c r="O45" s="18"/>
-      <c r="P45" s="26"/>
-      <c r="U45" s="26"/>
-      <c r="X45" s="26"/>
-      <c r="Y45" s="26"/>
-      <c r="Z45" s="26"/>
-      <c r="AA45" s="26"/>
-      <c r="AB45" s="26"/>
-      <c r="AC45" s="26"/>
-      <c r="AD45" s="41"/>
-      <c r="AE45" s="26"/>
-      <c r="AG45" s="2"/>
-      <c r="AH45" s="2"/>
-      <c r="AM45" s="2"/>
-      <c r="AO45" s="2"/>
-      <c r="AP45" s="17"/>
-      <c r="AR45" s="2"/>
-      <c r="AS45" s="12"/>
-      <c r="AT45" s="12"/>
-      <c r="AU45" s="12"/>
-      <c r="AV45" s="18"/>
-      <c r="AW45" s="18"/>
-      <c r="AX45" s="18"/>
+      <c r="A45" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="C45" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>211</v>
+      </c>
+      <c r="E45" t="s">
+        <v>188</v>
+      </c>
+      <c r="F45">
+        <v>1000</v>
+      </c>
+      <c r="G45">
+        <v>500</v>
+      </c>
+      <c r="H45" t="s">
+        <v>109</v>
+      </c>
+      <c r="I45" t="s">
+        <v>109</v>
+      </c>
+      <c r="J45" t="s">
+        <v>208</v>
+      </c>
+      <c r="K45" t="s">
+        <v>167</v>
+      </c>
+      <c r="L45" t="s">
+        <v>215</v>
+      </c>
+      <c r="M45" t="s">
+        <v>202</v>
+      </c>
+      <c r="N45" s="26">
+        <v>0</v>
+      </c>
+      <c r="O45" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P45" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q45">
+        <v>3</v>
+      </c>
+      <c r="R45">
+        <v>75</v>
+      </c>
+      <c r="S45">
+        <v>50</v>
+      </c>
+      <c r="T45">
+        <v>60</v>
+      </c>
+      <c r="U45" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V45">
+        <v>0</v>
+      </c>
+      <c r="W45">
+        <v>10</v>
+      </c>
+      <c r="X45" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y45" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z45" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA45" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB45" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC45" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD45" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE45" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF45" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG45" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH45" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI45">
+        <v>30</v>
+      </c>
+      <c r="AJ45" t="s">
+        <v>142</v>
+      </c>
+      <c r="AK45">
+        <v>5</v>
+      </c>
+      <c r="AL45">
+        <v>200</v>
+      </c>
+      <c r="AM45" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN45">
+        <v>1</v>
+      </c>
+      <c r="AO45" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP45" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ45">
+        <v>200</v>
+      </c>
+      <c r="AR45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS45" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT45" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU45" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV45" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW45" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX45" s="18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B46" s="31" t="s">
-        <v>284</v>
-      </c>
-      <c r="C46" s="11"/>
-      <c r="N46" s="26"/>
-      <c r="O46" s="18"/>
-      <c r="P46" s="26"/>
-      <c r="U46" s="26"/>
-      <c r="X46" s="26"/>
-      <c r="Y46" s="26"/>
-      <c r="Z46" s="26"/>
-      <c r="AA46" s="26"/>
-      <c r="AB46" s="26"/>
-      <c r="AC46" s="26"/>
-      <c r="AD46" s="41"/>
-      <c r="AE46" s="26"/>
-      <c r="AG46" s="2"/>
-      <c r="AH46" s="2"/>
-      <c r="AM46" s="2"/>
-      <c r="AO46" s="2"/>
-      <c r="AP46" s="17"/>
-      <c r="AR46" s="2"/>
-      <c r="AS46" s="12"/>
-      <c r="AT46" s="12"/>
-      <c r="AU46" s="12"/>
-      <c r="AV46" s="18"/>
-      <c r="AW46" s="18"/>
-      <c r="AX46" s="18"/>
+      <c r="A46" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="C46" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" t="s">
+        <v>211</v>
+      </c>
+      <c r="E46" t="s">
+        <v>188</v>
+      </c>
+      <c r="F46">
+        <v>1000</v>
+      </c>
+      <c r="G46">
+        <v>500</v>
+      </c>
+      <c r="H46" t="s">
+        <v>109</v>
+      </c>
+      <c r="I46" t="s">
+        <v>109</v>
+      </c>
+      <c r="J46" t="s">
+        <v>208</v>
+      </c>
+      <c r="K46" t="s">
+        <v>167</v>
+      </c>
+      <c r="L46" t="s">
+        <v>215</v>
+      </c>
+      <c r="M46" t="s">
+        <v>202</v>
+      </c>
+      <c r="N46" s="26">
+        <v>0</v>
+      </c>
+      <c r="O46" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P46" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q46">
+        <v>3</v>
+      </c>
+      <c r="R46">
+        <v>75</v>
+      </c>
+      <c r="S46">
+        <v>50</v>
+      </c>
+      <c r="T46">
+        <v>60</v>
+      </c>
+      <c r="U46" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>10</v>
+      </c>
+      <c r="X46" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y46" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z46" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA46" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB46" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC46" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD46" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE46" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF46" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG46" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH46" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI46">
+        <v>30</v>
+      </c>
+      <c r="AJ46" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK46">
+        <v>5</v>
+      </c>
+      <c r="AL46">
+        <v>200</v>
+      </c>
+      <c r="AM46" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN46">
+        <v>1</v>
+      </c>
+      <c r="AO46" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP46" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ46">
+        <v>200</v>
+      </c>
+      <c r="AR46" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS46" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT46" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU46" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV46" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW46" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX46" s="18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A47" s="34" t="s">
-        <v>285</v>
+        <v>349</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C47" s="11" t="b">
         <v>0</v>
@@ -7476,10 +7355,10 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AC47" s="26" t="s">
-        <v>156</v>
+        <v>346</v>
       </c>
       <c r="AD47" s="41">
-        <v>7.4999999999999997E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE47" s="26">
         <v>0.12</v>
@@ -7500,7 +7379,7 @@
         <v>115</v>
       </c>
       <c r="AK47">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AL47">
         <v>200</v>
@@ -7543,11 +7422,11 @@
       </c>
     </row>
     <row r="48" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
-        <v>288</v>
+      <c r="A48" s="40" t="s">
+        <v>282</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C48" s="11" t="b">
         <v>0</v>
@@ -7628,7 +7507,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="AC48" s="26" t="s">
-        <v>156</v>
+        <v>346</v>
       </c>
       <c r="AD48" s="41">
         <v>8.2199999999999995E-2</v>
@@ -7667,7 +7546,7 @@
         <v>166</v>
       </c>
       <c r="AP48" s="17">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="AQ48">
         <v>200</v>
@@ -7691,6 +7570,368 @@
         <v>1</v>
       </c>
       <c r="AX48" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A49" s="40"/>
+      <c r="C49" s="11"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="26"/>
+      <c r="U49" s="26"/>
+      <c r="X49" s="26"/>
+      <c r="Y49" s="26"/>
+      <c r="Z49" s="26"/>
+      <c r="AA49" s="26"/>
+      <c r="AB49" s="26"/>
+      <c r="AC49" s="26"/>
+      <c r="AD49" s="41"/>
+      <c r="AE49" s="26"/>
+      <c r="AG49" s="2"/>
+      <c r="AH49" s="2"/>
+      <c r="AM49" s="2"/>
+      <c r="AO49" s="2"/>
+      <c r="AP49" s="17"/>
+      <c r="AR49" s="2"/>
+      <c r="AS49" s="12"/>
+      <c r="AT49" s="12"/>
+      <c r="AU49" s="12"/>
+      <c r="AV49" s="18"/>
+      <c r="AW49" s="18"/>
+      <c r="AX49" s="18"/>
+    </row>
+    <row r="50" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="B50" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="C50" s="11"/>
+      <c r="N50" s="26"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="26"/>
+      <c r="U50" s="26"/>
+      <c r="X50" s="26"/>
+      <c r="Y50" s="26"/>
+      <c r="Z50" s="26"/>
+      <c r="AA50" s="26"/>
+      <c r="AB50" s="26"/>
+      <c r="AC50" s="26"/>
+      <c r="AD50" s="41"/>
+      <c r="AE50" s="26"/>
+      <c r="AG50" s="2"/>
+      <c r="AH50" s="2"/>
+      <c r="AM50" s="2"/>
+      <c r="AO50" s="2"/>
+      <c r="AP50" s="17"/>
+      <c r="AR50" s="2"/>
+      <c r="AS50" s="12"/>
+      <c r="AT50" s="12"/>
+      <c r="AU50" s="12"/>
+      <c r="AV50" s="18"/>
+      <c r="AW50" s="18"/>
+      <c r="AX50" s="18"/>
+    </row>
+    <row r="51" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A51" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="C51" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" t="s">
+        <v>211</v>
+      </c>
+      <c r="E51" t="s">
+        <v>188</v>
+      </c>
+      <c r="F51">
+        <v>1000</v>
+      </c>
+      <c r="G51">
+        <v>500</v>
+      </c>
+      <c r="H51" t="s">
+        <v>109</v>
+      </c>
+      <c r="I51" t="s">
+        <v>109</v>
+      </c>
+      <c r="J51" t="s">
+        <v>208</v>
+      </c>
+      <c r="K51" t="s">
+        <v>167</v>
+      </c>
+      <c r="L51" t="s">
+        <v>215</v>
+      </c>
+      <c r="M51" t="s">
+        <v>202</v>
+      </c>
+      <c r="N51" s="26">
+        <v>0</v>
+      </c>
+      <c r="O51" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P51" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q51">
+        <v>3</v>
+      </c>
+      <c r="R51">
+        <v>75</v>
+      </c>
+      <c r="S51">
+        <v>50</v>
+      </c>
+      <c r="T51">
+        <v>60</v>
+      </c>
+      <c r="U51" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V51">
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <v>10</v>
+      </c>
+      <c r="X51" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y51" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z51" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA51" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB51" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC51" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD51" s="41">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AE51" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF51" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG51" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH51" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI51">
+        <v>30</v>
+      </c>
+      <c r="AJ51" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK51">
+        <v>5</v>
+      </c>
+      <c r="AL51">
+        <v>200</v>
+      </c>
+      <c r="AM51" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN51">
+        <v>1</v>
+      </c>
+      <c r="AO51" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP51" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ51">
+        <v>200</v>
+      </c>
+      <c r="AR51" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS51" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT51" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU51" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV51" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW51" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX51" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A52" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="C52" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" t="s">
+        <v>211</v>
+      </c>
+      <c r="E52" t="s">
+        <v>188</v>
+      </c>
+      <c r="F52">
+        <v>1000</v>
+      </c>
+      <c r="G52">
+        <v>500</v>
+      </c>
+      <c r="H52" t="s">
+        <v>109</v>
+      </c>
+      <c r="I52" t="s">
+        <v>109</v>
+      </c>
+      <c r="J52" t="s">
+        <v>208</v>
+      </c>
+      <c r="K52" t="s">
+        <v>167</v>
+      </c>
+      <c r="L52" t="s">
+        <v>215</v>
+      </c>
+      <c r="M52" t="s">
+        <v>202</v>
+      </c>
+      <c r="N52" s="26">
+        <v>0</v>
+      </c>
+      <c r="O52" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P52" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q52">
+        <v>3</v>
+      </c>
+      <c r="R52">
+        <v>75</v>
+      </c>
+      <c r="S52">
+        <v>50</v>
+      </c>
+      <c r="T52">
+        <v>60</v>
+      </c>
+      <c r="U52" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V52">
+        <v>0</v>
+      </c>
+      <c r="W52">
+        <v>10</v>
+      </c>
+      <c r="X52" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y52" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z52" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA52" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB52" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC52" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD52" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE52" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF52" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG52" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH52" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI52">
+        <v>30</v>
+      </c>
+      <c r="AJ52" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK52">
+        <v>5</v>
+      </c>
+      <c r="AL52">
+        <v>200</v>
+      </c>
+      <c r="AM52" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN52">
+        <v>1</v>
+      </c>
+      <c r="AO52" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP52" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ52">
+        <v>200</v>
+      </c>
+      <c r="AR52" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS52" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT52" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU52" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV52" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW52" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX52" s="18" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7709,82 +7950,82 @@
     <mergeCell ref="H4:J4"/>
   </mergeCells>
   <dataValidations count="21">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM9 AM13:AM48">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM9 AM13:AM52">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH9 AH13:AH48">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH9 AH13:AH52">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AG9 AG13:AG48">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AG9 AG13:AG52">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR6:AR9 AR13:AR48">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR6:AR9 AR13:AR52">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O9 C6:C10 O13:O48 C13:C48">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O9 C6:C10 C13:C52 O13:O52">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="AA6:AA9 U6:U9 U13:U48 AA13:AA48">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="AA6:AA9 U6:U9 AA13:AA52 U13:U52">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="V6:W9 V13:W48">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="V6:W9 V13:W52">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Z9 AB6:AB9 AD6:AD9 AD13:AD48 AB13:AB48 X13:Z48">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Z9 AB6:AB9 AD6:AD9 X13:Z52 AB13:AB52 AD13:AD52">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AI6:AI9 AI13:AI48">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AI6:AI9 AI13:AI52">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AS6:AT9 AS13:AT48">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AS6:AT9 AS13:AT52">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AU6:AU9 AU13:AU48">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AU6:AU9 AU13:AU52">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AE6:AE9 AE13:AE48">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AE6:AE9 AE13:AE52">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AK6:AK9 AK13:AK48">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AK6:AK9 AK13:AK52">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL9 AL13:AL48">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL9 AL13:AL52">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN13:AN48">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN13:AN52">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AC6:AC9 AC13:AC48"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV6:AX9 AV13:AX48">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AC6:AC9 AC13:AC52"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV6:AX9 AV13:AX52">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO9 AO13:AO48">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO9 AO13:AO52">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP9 AP13:AP48">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP9 AP13:AP52">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="R6:R9 R13:R48">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="R6:R9 R13:R52">
       <formula1>35</formula1>
       <formula2>80</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:I9 H13:I48">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:I9 H13:I52">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -7797,37 +8038,37 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$57:$A$61</xm:f>
           </x14:formula1>
-          <xm:sqref>K6:K9 K13:K48</xm:sqref>
+          <xm:sqref>K6:K9 K13:K52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$64:$A$71</xm:f>
           </x14:formula1>
-          <xm:sqref>L6:L9 L13:L48</xm:sqref>
+          <xm:sqref>L6:L9 L13:L52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$45:$A$52</xm:f>
           </x14:formula1>
-          <xm:sqref>E6:E9 E13:E48</xm:sqref>
+          <xm:sqref>E6:E9 E13:E52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$29:$A$42</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:D9 D13:D48</xm:sqref>
+          <xm:sqref>D6:D9 D13:D52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$21:$A$24</xm:f>
           </x14:formula1>
-          <xm:sqref>J6:J9 J13:J48</xm:sqref>
+          <xm:sqref>J6:J9 J13:J52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$74:$A$77</xm:f>
           </x14:formula1>
-          <xm:sqref>M6:M9 M13:M48</xm:sqref>
+          <xm:sqref>M6:M9 M13:M52</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Analysis for new M1 report
</commit_message>
<xml_diff>
--- a/IO_M1_new/RunControl_M1_new.xlsx
+++ b/IO_M1_new/RunControl_M1_new.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="358">
   <si>
     <t>Sheet #</t>
   </si>
@@ -1133,6 +1133,15 @@
   </si>
   <si>
     <t>A1F075_O30pA5_cap</t>
+  </si>
+  <si>
+    <t>A1F075_soa4.1</t>
+  </si>
+  <si>
+    <t>75% initial Funding; SOA smoothing: open 15-year cp; 5-year asset smoothing, DR 5.9%, ir 5.9%, sd 12%; Preset MA</t>
+  </si>
+  <si>
+    <t>A1F075_soa2.1</t>
   </si>
 </sst>
 </file>
@@ -1387,10 +1396,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1399,13 +1405,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2052,13 +2061,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX52"/>
+  <dimension ref="A1:AX54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
+      <selection pane="bottomRight" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2251,61 +2260,61 @@
       </c>
     </row>
     <row r="4" spans="1:50" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43" t="s">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="43"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="27"/>
       <c r="G4" s="27"/>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="44" t="s">
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="L4" s="44"/>
+      <c r="L4" s="43"/>
       <c r="M4" s="28"/>
-      <c r="N4" s="45" t="s">
+      <c r="N4" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="O4" s="45"/>
-      <c r="P4" s="44" t="s">
+      <c r="O4" s="44"/>
+      <c r="P4" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="Q4" s="44"/>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
-      <c r="V4" s="44"/>
-      <c r="W4" s="44"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
       <c r="X4" s="29"/>
       <c r="Y4" s="29"/>
-      <c r="Z4" s="45" t="s">
+      <c r="Z4" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="AA4" s="45"/>
-      <c r="AB4" s="45"/>
-      <c r="AC4" s="47" t="s">
+      <c r="AA4" s="44"/>
+      <c r="AB4" s="44"/>
+      <c r="AC4" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="AD4" s="47"/>
-      <c r="AE4" s="47"/>
+      <c r="AD4" s="42"/>
+      <c r="AE4" s="42"/>
       <c r="AF4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AG4" s="42" t="s">
+      <c r="AG4" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="AH4" s="42"/>
-      <c r="AI4" s="42"/>
+      <c r="AH4" s="45"/>
+      <c r="AI4" s="45"/>
       <c r="AJ4" s="21" t="s">
         <v>70</v>
       </c>
@@ -2313,17 +2322,17 @@
       <c r="AL4" s="21"/>
       <c r="AM4" s="21"/>
       <c r="AN4" s="21"/>
-      <c r="AO4" s="47" t="s">
+      <c r="AO4" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="AP4" s="47"/>
-      <c r="AQ4" s="47"/>
-      <c r="AR4" s="48" t="s">
+      <c r="AP4" s="42"/>
+      <c r="AQ4" s="42"/>
+      <c r="AR4" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="AS4" s="48"/>
-      <c r="AT4" s="48"/>
-      <c r="AU4" s="48"/>
+      <c r="AS4" s="46"/>
+      <c r="AT4" s="46"/>
+      <c r="AU4" s="46"/>
       <c r="AV4" s="15"/>
       <c r="AW4" s="22"/>
       <c r="AX4" s="20"/>
@@ -3129,7 +3138,7 @@
         <v>226</v>
       </c>
       <c r="C14" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
         <v>211</v>
@@ -3281,7 +3290,7 @@
         <v>229</v>
       </c>
       <c r="C15" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="s">
         <v>211</v>
@@ -3433,7 +3442,7 @@
         <v>231</v>
       </c>
       <c r="C16" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
         <v>211</v>
@@ -3585,7 +3594,7 @@
         <v>233</v>
       </c>
       <c r="C17" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
         <v>211</v>
@@ -3737,7 +3746,7 @@
         <v>235</v>
       </c>
       <c r="C18" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="s">
         <v>211</v>
@@ -3889,7 +3898,7 @@
         <v>237</v>
       </c>
       <c r="C19" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
         <v>211</v>
@@ -4041,7 +4050,7 @@
         <v>239</v>
       </c>
       <c r="C20" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
         <v>211</v>
@@ -4193,7 +4202,7 @@
         <v>241</v>
       </c>
       <c r="C21" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>211</v>
@@ -4345,7 +4354,7 @@
         <v>243</v>
       </c>
       <c r="C22" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="s">
         <v>211</v>
@@ -4497,7 +4506,7 @@
         <v>245</v>
       </c>
       <c r="C23" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D23" t="s">
         <v>211</v>
@@ -4649,7 +4658,7 @@
         <v>247</v>
       </c>
       <c r="C24" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="s">
         <v>211</v>
@@ -4829,7 +4838,7 @@
         <v>249</v>
       </c>
       <c r="C26" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
         <v>211</v>
@@ -4981,7 +4990,7 @@
         <v>251</v>
       </c>
       <c r="C27" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>211</v>
@@ -5133,7 +5142,7 @@
         <v>253</v>
       </c>
       <c r="C28" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
         <v>211</v>
@@ -5285,7 +5294,7 @@
         <v>255</v>
       </c>
       <c r="C29" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29" t="s">
         <v>211</v>
@@ -5437,7 +5446,7 @@
         <v>257</v>
       </c>
       <c r="C30" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
         <v>211</v>
@@ -5589,7 +5598,7 @@
         <v>351</v>
       </c>
       <c r="C31" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" t="s">
         <v>211</v>
@@ -5741,7 +5750,7 @@
         <v>259</v>
       </c>
       <c r="C32" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
         <v>211</v>
@@ -5920,7 +5929,7 @@
         <v>261</v>
       </c>
       <c r="C34" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" t="s">
         <v>211</v>
@@ -6073,7 +6082,7 @@
         <v>263</v>
       </c>
       <c r="C35" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" t="s">
         <v>211</v>
@@ -6193,7 +6202,7 @@
         <v>0.75</v>
       </c>
       <c r="AQ35" s="25">
-        <f t="shared" ref="AQ35:AQ37" si="0">225068282*0.75</f>
+        <f t="shared" ref="AQ35:AQ39" si="0">225068282*0.75</f>
         <v>168801211.5</v>
       </c>
       <c r="AR35" s="2" t="s">
@@ -6219,14 +6228,14 @@
       </c>
     </row>
     <row r="36" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
-        <v>266</v>
+      <c r="A36" t="s">
+        <v>357</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C36" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="s">
         <v>211</v>
@@ -6301,13 +6310,13 @@
         <v>0.01</v>
       </c>
       <c r="AB36" s="26">
-        <v>5.8999999999999997E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AC36" s="26" t="s">
         <v>156</v>
       </c>
       <c r="AD36" s="41">
-        <v>8.2199999999999995E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AE36" s="26">
         <v>0.12</v>
@@ -6372,14 +6381,14 @@
       </c>
     </row>
     <row r="37" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>269</v>
+      <c r="A37" s="37" t="s">
+        <v>266</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C37" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37" t="s">
         <v>211</v>
@@ -6460,7 +6469,7 @@
         <v>156</v>
       </c>
       <c r="AD37" s="41">
-        <v>6.6199999999999995E-2</v>
+        <v>8.2199999999999995E-2</v>
       </c>
       <c r="AE37" s="26">
         <v>0.12</v>
@@ -6503,7 +6512,7 @@
         <v>168801211.5</v>
       </c>
       <c r="AR37" s="2" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="AS37" s="12">
         <v>0.25</v>
@@ -6525,40 +6534,164 @@
       </c>
     </row>
     <row r="38" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B38" s="19"/>
-      <c r="C38" s="11"/>
-      <c r="N38" s="26"/>
-      <c r="O38" s="18"/>
-      <c r="P38" s="26"/>
-      <c r="U38" s="26"/>
-      <c r="X38" s="26"/>
-      <c r="Y38" s="26"/>
-      <c r="Z38" s="26"/>
-      <c r="AA38" s="26"/>
-      <c r="AB38" s="26"/>
-      <c r="AC38" s="26"/>
-      <c r="AD38" s="41"/>
-      <c r="AE38" s="26"/>
-      <c r="AG38" s="2"/>
-      <c r="AH38" s="2"/>
-      <c r="AM38" s="2"/>
-      <c r="AO38" s="2"/>
-      <c r="AP38" s="17"/>
-      <c r="AQ38" s="25"/>
-      <c r="AR38" s="2"/>
-      <c r="AS38" s="12"/>
-      <c r="AT38" s="12"/>
-      <c r="AU38" s="12"/>
-      <c r="AV38" s="18"/>
-      <c r="AW38" s="18"/>
-      <c r="AX38" s="18"/>
+      <c r="A38" t="s">
+        <v>269</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="C38" s="11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="s">
+        <v>211</v>
+      </c>
+      <c r="E38" t="s">
+        <v>188</v>
+      </c>
+      <c r="F38">
+        <v>1000</v>
+      </c>
+      <c r="G38">
+        <v>500</v>
+      </c>
+      <c r="H38" t="s">
+        <v>109</v>
+      </c>
+      <c r="I38" t="s">
+        <v>109</v>
+      </c>
+      <c r="J38" t="s">
+        <v>208</v>
+      </c>
+      <c r="K38" t="s">
+        <v>167</v>
+      </c>
+      <c r="L38" t="s">
+        <v>215</v>
+      </c>
+      <c r="M38" t="s">
+        <v>202</v>
+      </c>
+      <c r="N38" s="26">
+        <v>0</v>
+      </c>
+      <c r="O38" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P38" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q38">
+        <v>3</v>
+      </c>
+      <c r="R38">
+        <v>75</v>
+      </c>
+      <c r="S38">
+        <v>50</v>
+      </c>
+      <c r="T38">
+        <v>60</v>
+      </c>
+      <c r="U38" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>10</v>
+      </c>
+      <c r="X38" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y38" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z38" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA38" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB38" s="26">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AC38" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD38" s="41">
+        <v>6.6199999999999995E-2</v>
+      </c>
+      <c r="AE38" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF38" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG38" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH38" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI38">
+        <v>15</v>
+      </c>
+      <c r="AJ38" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK38">
+        <v>5</v>
+      </c>
+      <c r="AL38">
+        <v>200</v>
+      </c>
+      <c r="AM38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN38">
+        <v>1</v>
+      </c>
+      <c r="AO38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP38" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ38" s="25">
+        <f t="shared" si="0"/>
+        <v>168801211.5</v>
+      </c>
+      <c r="AR38" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS38" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT38" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU38" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV38" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW38" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX38" s="18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>259</v>
+        <v>356</v>
       </c>
       <c r="C39" s="11" t="b">
         <v>1</v>
@@ -6636,13 +6769,13 @@
         <v>0.01</v>
       </c>
       <c r="AB39" s="26">
-        <v>7.4999999999999997E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="AC39" s="26" t="s">
         <v>156</v>
       </c>
       <c r="AD39" s="41">
-        <v>8.2199999999999995E-2</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="AE39" s="26">
         <v>0.12</v>
@@ -6657,7 +6790,7 @@
         <v>348</v>
       </c>
       <c r="AI39">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="AJ39" t="s">
         <v>115</v>
@@ -6675,19 +6808,20 @@
         <v>1</v>
       </c>
       <c r="AO39" s="2" t="s">
-        <v>166</v>
+        <v>114</v>
       </c>
       <c r="AP39" s="17">
         <v>0.75</v>
       </c>
-      <c r="AQ39">
-        <v>200</v>
+      <c r="AQ39" s="25">
+        <f t="shared" si="0"/>
+        <v>168801211.5</v>
       </c>
       <c r="AR39" s="2" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="AS39" s="12">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="AT39" s="12">
         <v>0.14499999999999999</v>
@@ -6706,681 +6840,558 @@
       </c>
     </row>
     <row r="40" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
+      <c r="B40" s="19"/>
+      <c r="C40" s="11"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="26"/>
+      <c r="U40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="26"/>
+      <c r="Z40" s="26"/>
+      <c r="AA40" s="26"/>
+      <c r="AB40" s="26"/>
+      <c r="AC40" s="26"/>
+      <c r="AD40" s="41"/>
+      <c r="AE40" s="26"/>
+      <c r="AG40" s="2"/>
+      <c r="AH40" s="2"/>
+      <c r="AM40" s="2"/>
+      <c r="AO40" s="2"/>
+      <c r="AP40" s="17"/>
+      <c r="AQ40" s="25"/>
+      <c r="AR40" s="2"/>
+      <c r="AS40" s="12"/>
+      <c r="AT40" s="12"/>
+      <c r="AU40" s="12"/>
+      <c r="AV40" s="18"/>
+      <c r="AW40" s="18"/>
+      <c r="AX40" s="18"/>
+    </row>
+    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>354</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="C41" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>211</v>
+      </c>
+      <c r="E41" t="s">
+        <v>188</v>
+      </c>
+      <c r="F41">
+        <v>1000</v>
+      </c>
+      <c r="G41">
+        <v>500</v>
+      </c>
+      <c r="H41" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" t="s">
+        <v>109</v>
+      </c>
+      <c r="J41" t="s">
+        <v>208</v>
+      </c>
+      <c r="K41" t="s">
+        <v>167</v>
+      </c>
+      <c r="L41" t="s">
+        <v>215</v>
+      </c>
+      <c r="M41" t="s">
+        <v>202</v>
+      </c>
+      <c r="N41" s="26">
+        <v>0</v>
+      </c>
+      <c r="O41" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P41" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q41">
+        <v>3</v>
+      </c>
+      <c r="R41">
+        <v>75</v>
+      </c>
+      <c r="S41">
+        <v>50</v>
+      </c>
+      <c r="T41">
+        <v>60</v>
+      </c>
+      <c r="U41" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V41">
+        <v>0</v>
+      </c>
+      <c r="W41">
+        <v>10</v>
+      </c>
+      <c r="X41" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y41" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z41" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA41" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB41" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC41" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD41" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE41" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG41" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH41" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI41">
+        <v>30</v>
+      </c>
+      <c r="AJ41" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK41">
+        <v>5</v>
+      </c>
+      <c r="AL41">
+        <v>200</v>
+      </c>
+      <c r="AM41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN41">
+        <v>1</v>
+      </c>
+      <c r="AO41" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP41" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ41">
+        <v>200</v>
+      </c>
+      <c r="AR41" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AS41" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="AT41" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU41" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV41" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW41" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX41" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A42" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="B40" s="19" t="s">
+      <c r="B42" s="19" t="s">
         <v>261</v>
       </c>
-      <c r="C40" s="11" t="b">
+      <c r="C42" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>211</v>
+      </c>
+      <c r="E42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F42">
+        <v>1000</v>
+      </c>
+      <c r="G42">
+        <v>500</v>
+      </c>
+      <c r="H42" t="s">
+        <v>109</v>
+      </c>
+      <c r="I42" t="s">
+        <v>109</v>
+      </c>
+      <c r="J42" t="s">
+        <v>208</v>
+      </c>
+      <c r="K42" t="s">
+        <v>167</v>
+      </c>
+      <c r="L42" t="s">
+        <v>215</v>
+      </c>
+      <c r="M42" t="s">
+        <v>202</v>
+      </c>
+      <c r="N42" s="26">
+        <v>0</v>
+      </c>
+      <c r="O42" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P42" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q42">
+        <v>3</v>
+      </c>
+      <c r="R42">
+        <v>75</v>
+      </c>
+      <c r="S42">
+        <v>50</v>
+      </c>
+      <c r="T42">
+        <v>60</v>
+      </c>
+      <c r="U42" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>10</v>
+      </c>
+      <c r="X42" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y42" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z42" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA42" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB42" s="26">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="AC42" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD42" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE42" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF42" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG42" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH42" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI42">
+        <v>15</v>
+      </c>
+      <c r="AJ42" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK42">
+        <v>5</v>
+      </c>
+      <c r="AL42">
+        <v>200</v>
+      </c>
+      <c r="AM42" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN42">
         <v>1</v>
       </c>
-      <c r="D40" t="s">
-        <v>211</v>
-      </c>
-      <c r="E40" t="s">
-        <v>188</v>
-      </c>
-      <c r="F40">
-        <v>1000</v>
-      </c>
-      <c r="G40">
-        <v>500</v>
-      </c>
-      <c r="H40" t="s">
-        <v>109</v>
-      </c>
-      <c r="I40" t="s">
-        <v>109</v>
-      </c>
-      <c r="J40" t="s">
-        <v>208</v>
-      </c>
-      <c r="K40" t="s">
-        <v>167</v>
-      </c>
-      <c r="L40" t="s">
-        <v>215</v>
-      </c>
-      <c r="M40" t="s">
-        <v>202</v>
-      </c>
-      <c r="N40" s="26">
-        <v>0</v>
-      </c>
-      <c r="O40" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P40" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q40">
-        <v>3</v>
-      </c>
-      <c r="R40">
-        <v>75</v>
-      </c>
-      <c r="S40">
-        <v>50</v>
-      </c>
-      <c r="T40">
-        <v>60</v>
-      </c>
-      <c r="U40" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V40">
-        <v>0</v>
-      </c>
-      <c r="W40">
-        <v>10</v>
-      </c>
-      <c r="X40" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y40" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z40" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA40" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB40" s="26">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="AC40" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD40" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE40" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF40" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG40" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH40" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI40">
-        <v>15</v>
-      </c>
-      <c r="AJ40" t="s">
-        <v>115</v>
-      </c>
-      <c r="AK40">
-        <v>5</v>
-      </c>
-      <c r="AL40">
-        <v>200</v>
-      </c>
-      <c r="AM40" s="2" t="s">
+      <c r="AO42" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="AN40">
-        <v>1</v>
-      </c>
-      <c r="AO40" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AP40" s="17">
+      <c r="AP42" s="17">
         <v>0.75</v>
       </c>
-      <c r="AQ40" s="25">
+      <c r="AQ42" s="25">
         <f>225068282*0.75</f>
         <v>168801211.5</v>
       </c>
-      <c r="AR40" s="2" t="s">
+      <c r="AR42" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="AS40" s="12">
+      <c r="AS42" s="12">
         <v>0.2</v>
       </c>
-      <c r="AT40" s="12">
+      <c r="AT42" s="12">
         <v>0.14499999999999999</v>
       </c>
-      <c r="AU40" s="12">
+      <c r="AU42" s="12">
         <v>0.05</v>
       </c>
-      <c r="AV40" s="18" t="b">
+      <c r="AV42" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="AW40" s="18" t="b">
+      <c r="AW42" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="AX40" s="18" t="b">
+      <c r="AX42" s="18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A41" s="37" t="s">
-        <v>353</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="C41" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" t="s">
-        <v>211</v>
-      </c>
-      <c r="E41" t="s">
-        <v>188</v>
-      </c>
-      <c r="F41">
-        <v>1000</v>
-      </c>
-      <c r="G41">
-        <v>500</v>
-      </c>
-      <c r="H41" t="s">
-        <v>109</v>
-      </c>
-      <c r="I41" t="s">
-        <v>109</v>
-      </c>
-      <c r="J41" t="s">
-        <v>208</v>
-      </c>
-      <c r="K41" t="s">
-        <v>167</v>
-      </c>
-      <c r="L41" t="s">
-        <v>215</v>
-      </c>
-      <c r="M41" t="s">
-        <v>202</v>
-      </c>
-      <c r="N41" s="26">
-        <v>0</v>
-      </c>
-      <c r="O41" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P41" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q41">
-        <v>3</v>
-      </c>
-      <c r="R41">
-        <v>75</v>
-      </c>
-      <c r="S41">
-        <v>50</v>
-      </c>
-      <c r="T41">
-        <v>60</v>
-      </c>
-      <c r="U41" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V41">
-        <v>0</v>
-      </c>
-      <c r="W41">
-        <v>10</v>
-      </c>
-      <c r="X41" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y41" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z41" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA41" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB41" s="26">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="AC41" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD41" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE41" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF41" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG41" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH41" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI41">
-        <v>15</v>
-      </c>
-      <c r="AJ41" t="s">
-        <v>115</v>
-      </c>
-      <c r="AK41">
-        <v>5</v>
-      </c>
-      <c r="AL41">
-        <v>200</v>
-      </c>
-      <c r="AM41" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN41">
-        <v>1</v>
-      </c>
-      <c r="AO41" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AP41" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ41" s="25">
-        <f t="shared" ref="AQ41" si="1">225068282*0.75</f>
-        <v>168801211.5</v>
-      </c>
-      <c r="AR41" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="AS41" s="12">
-        <v>0.2</v>
-      </c>
-      <c r="AT41" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU41" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV41" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW41" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX41" s="18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="C42" s="11"/>
-      <c r="N42" s="26"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="26"/>
-      <c r="U42" s="26"/>
-      <c r="X42" s="26"/>
-      <c r="Y42" s="26"/>
-      <c r="Z42" s="26"/>
-      <c r="AA42" s="26"/>
-      <c r="AB42" s="26"/>
-      <c r="AC42" s="26"/>
-      <c r="AD42" s="41"/>
-      <c r="AE42" s="26"/>
-      <c r="AG42" s="2"/>
-      <c r="AH42" s="2"/>
-      <c r="AM42" s="2"/>
-      <c r="AO42" s="2"/>
-      <c r="AP42" s="17"/>
-      <c r="AR42" s="2"/>
-      <c r="AS42" s="12"/>
-      <c r="AT42" s="12"/>
-      <c r="AU42" s="12"/>
-      <c r="AV42" s="18"/>
-      <c r="AW42" s="18"/>
-      <c r="AX42" s="18"/>
     </row>
     <row r="43" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B43" s="39" t="s">
-        <v>273</v>
-      </c>
-      <c r="C43" s="11"/>
-      <c r="N43" s="26"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="26"/>
-      <c r="U43" s="26"/>
-      <c r="X43" s="26"/>
-      <c r="Y43" s="26"/>
-      <c r="Z43" s="26"/>
-      <c r="AA43" s="26"/>
-      <c r="AB43" s="26"/>
-      <c r="AC43" s="26"/>
-      <c r="AD43" s="41"/>
-      <c r="AE43" s="26"/>
-      <c r="AG43" s="2"/>
-      <c r="AH43" s="2"/>
-      <c r="AM43" s="2"/>
-      <c r="AO43" s="2"/>
-      <c r="AP43" s="17"/>
-      <c r="AR43" s="2"/>
-      <c r="AS43" s="12"/>
-      <c r="AT43" s="12"/>
-      <c r="AU43" s="12"/>
-      <c r="AV43" s="18"/>
-      <c r="AW43" s="18"/>
-      <c r="AX43" s="18"/>
+      <c r="A43" s="37" t="s">
+        <v>353</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="C43" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>211</v>
+      </c>
+      <c r="E43" t="s">
+        <v>188</v>
+      </c>
+      <c r="F43">
+        <v>1000</v>
+      </c>
+      <c r="G43">
+        <v>500</v>
+      </c>
+      <c r="H43" t="s">
+        <v>109</v>
+      </c>
+      <c r="I43" t="s">
+        <v>109</v>
+      </c>
+      <c r="J43" t="s">
+        <v>208</v>
+      </c>
+      <c r="K43" t="s">
+        <v>167</v>
+      </c>
+      <c r="L43" t="s">
+        <v>215</v>
+      </c>
+      <c r="M43" t="s">
+        <v>202</v>
+      </c>
+      <c r="N43" s="26">
+        <v>0</v>
+      </c>
+      <c r="O43" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P43" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q43">
+        <v>3</v>
+      </c>
+      <c r="R43">
+        <v>75</v>
+      </c>
+      <c r="S43">
+        <v>50</v>
+      </c>
+      <c r="T43">
+        <v>60</v>
+      </c>
+      <c r="U43" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V43">
+        <v>0</v>
+      </c>
+      <c r="W43">
+        <v>10</v>
+      </c>
+      <c r="X43" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y43" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z43" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA43" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB43" s="26">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AC43" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD43" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE43" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF43" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG43" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH43" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI43">
+        <v>15</v>
+      </c>
+      <c r="AJ43" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK43">
+        <v>5</v>
+      </c>
+      <c r="AL43">
+        <v>200</v>
+      </c>
+      <c r="AM43" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN43">
+        <v>1</v>
+      </c>
+      <c r="AO43" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AP43" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ43" s="25">
+        <f t="shared" ref="AQ43" si="1">225068282*0.75</f>
+        <v>168801211.5</v>
+      </c>
+      <c r="AR43" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="AS43" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="AT43" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU43" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV43" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW43" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX43" s="18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>274</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="C44" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
-        <v>211</v>
-      </c>
-      <c r="E44" t="s">
-        <v>188</v>
-      </c>
-      <c r="F44">
-        <v>1000</v>
-      </c>
-      <c r="G44">
-        <v>500</v>
-      </c>
-      <c r="H44" t="s">
-        <v>109</v>
-      </c>
-      <c r="I44" t="s">
-        <v>109</v>
-      </c>
-      <c r="J44" t="s">
-        <v>208</v>
-      </c>
-      <c r="K44" t="s">
-        <v>167</v>
-      </c>
-      <c r="L44" t="s">
-        <v>215</v>
-      </c>
-      <c r="M44" t="s">
-        <v>202</v>
-      </c>
-      <c r="N44" s="26">
-        <v>0</v>
-      </c>
-      <c r="O44" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P44" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q44">
-        <v>3</v>
-      </c>
-      <c r="R44">
-        <v>75</v>
-      </c>
-      <c r="S44">
-        <v>50</v>
-      </c>
-      <c r="T44">
-        <v>60</v>
-      </c>
-      <c r="U44" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V44">
-        <v>0</v>
-      </c>
-      <c r="W44">
-        <v>10</v>
-      </c>
-      <c r="X44" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y44" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z44" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA44" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB44" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC44" s="26" t="s">
-        <v>346</v>
-      </c>
-      <c r="AD44" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE44" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF44" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG44" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH44" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AI44">
-        <v>1</v>
-      </c>
-      <c r="AJ44" t="s">
-        <v>142</v>
-      </c>
-      <c r="AK44">
-        <v>5</v>
-      </c>
-      <c r="AL44">
-        <v>200</v>
-      </c>
-      <c r="AM44" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN44">
-        <v>1</v>
-      </c>
-      <c r="AO44" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP44" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ44">
-        <v>200</v>
-      </c>
-      <c r="AR44" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS44" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT44" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU44" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV44" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW44" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX44" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="C44" s="11"/>
+      <c r="N44" s="26"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="26"/>
+      <c r="U44" s="26"/>
+      <c r="X44" s="26"/>
+      <c r="Y44" s="26"/>
+      <c r="Z44" s="26"/>
+      <c r="AA44" s="26"/>
+      <c r="AB44" s="26"/>
+      <c r="AC44" s="26"/>
+      <c r="AD44" s="41"/>
+      <c r="AE44" s="26"/>
+      <c r="AG44" s="2"/>
+      <c r="AH44" s="2"/>
+      <c r="AM44" s="2"/>
+      <c r="AO44" s="2"/>
+      <c r="AP44" s="17"/>
+      <c r="AR44" s="2"/>
+      <c r="AS44" s="12"/>
+      <c r="AT44" s="12"/>
+      <c r="AU44" s="12"/>
+      <c r="AV44" s="18"/>
+      <c r="AW44" s="18"/>
+      <c r="AX44" s="18"/>
     </row>
     <row r="45" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A45" s="34" t="s">
-        <v>276</v>
-      </c>
-      <c r="B45" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="C45" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>211</v>
-      </c>
-      <c r="E45" t="s">
-        <v>188</v>
-      </c>
-      <c r="F45">
-        <v>1000</v>
-      </c>
-      <c r="G45">
-        <v>500</v>
-      </c>
-      <c r="H45" t="s">
-        <v>109</v>
-      </c>
-      <c r="I45" t="s">
-        <v>109</v>
-      </c>
-      <c r="J45" t="s">
-        <v>208</v>
-      </c>
-      <c r="K45" t="s">
-        <v>167</v>
-      </c>
-      <c r="L45" t="s">
-        <v>215</v>
-      </c>
-      <c r="M45" t="s">
-        <v>202</v>
-      </c>
-      <c r="N45" s="26">
-        <v>0</v>
-      </c>
-      <c r="O45" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P45" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q45">
-        <v>3</v>
-      </c>
-      <c r="R45">
-        <v>75</v>
-      </c>
-      <c r="S45">
-        <v>50</v>
-      </c>
-      <c r="T45">
-        <v>60</v>
-      </c>
-      <c r="U45" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V45">
-        <v>0</v>
-      </c>
-      <c r="W45">
-        <v>10</v>
-      </c>
-      <c r="X45" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y45" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z45" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA45" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB45" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC45" s="26" t="s">
-        <v>346</v>
-      </c>
-      <c r="AD45" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE45" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF45" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG45" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH45" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI45">
-        <v>30</v>
-      </c>
-      <c r="AJ45" t="s">
-        <v>142</v>
-      </c>
-      <c r="AK45">
-        <v>5</v>
-      </c>
-      <c r="AL45">
-        <v>200</v>
-      </c>
-      <c r="AM45" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN45">
-        <v>1</v>
-      </c>
-      <c r="AO45" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP45" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ45">
-        <v>200</v>
-      </c>
-      <c r="AR45" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS45" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT45" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU45" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV45" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW45" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX45" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="B45" s="39" t="s">
+        <v>273</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="N45" s="26"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="26"/>
+      <c r="U45" s="26"/>
+      <c r="X45" s="26"/>
+      <c r="Y45" s="26"/>
+      <c r="Z45" s="26"/>
+      <c r="AA45" s="26"/>
+      <c r="AB45" s="26"/>
+      <c r="AC45" s="26"/>
+      <c r="AD45" s="41"/>
+      <c r="AE45" s="26"/>
+      <c r="AG45" s="2"/>
+      <c r="AH45" s="2"/>
+      <c r="AM45" s="2"/>
+      <c r="AO45" s="2"/>
+      <c r="AP45" s="17"/>
+      <c r="AR45" s="2"/>
+      <c r="AS45" s="12"/>
+      <c r="AT45" s="12"/>
+      <c r="AU45" s="12"/>
+      <c r="AV45" s="18"/>
+      <c r="AW45" s="18"/>
+      <c r="AX45" s="18"/>
     </row>
     <row r="46" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A46" s="34" t="s">
-        <v>278</v>
+      <c r="A46" t="s">
+        <v>274</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C46" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="s">
         <v>211</v>
@@ -7473,13 +7484,13 @@
         <v>158</v>
       </c>
       <c r="AH46" s="2" t="s">
-        <v>348</v>
+        <v>179</v>
       </c>
       <c r="AI46">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="AJ46" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="AK46">
         <v>5</v>
@@ -7526,13 +7537,13 @@
     </row>
     <row r="47" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A47" s="34" t="s">
-        <v>349</v>
+        <v>276</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C47" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D47" t="s">
         <v>211</v>
@@ -7631,10 +7642,10 @@
         <v>30</v>
       </c>
       <c r="AJ47" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="AK47">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AL47">
         <v>200</v>
@@ -7677,14 +7688,14 @@
       </c>
     </row>
     <row r="48" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A48" s="40" t="s">
-        <v>282</v>
+      <c r="A48" s="34" t="s">
+        <v>278</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C48" s="11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48" t="s">
         <v>211</v>
@@ -7801,7 +7812,7 @@
         <v>166</v>
       </c>
       <c r="AP48" s="17">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AQ48">
         <v>200</v>
@@ -7829,458 +7840,762 @@
       </c>
     </row>
     <row r="49" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A49" s="40"/>
-      <c r="C49" s="11"/>
-      <c r="N49" s="26"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="26"/>
-      <c r="U49" s="26"/>
-      <c r="X49" s="26"/>
-      <c r="Y49" s="26"/>
-      <c r="Z49" s="26"/>
-      <c r="AA49" s="26"/>
-      <c r="AB49" s="26"/>
-      <c r="AC49" s="26"/>
-      <c r="AD49" s="41"/>
-      <c r="AE49" s="26"/>
-      <c r="AG49" s="2"/>
-      <c r="AH49" s="2"/>
-      <c r="AM49" s="2"/>
-      <c r="AO49" s="2"/>
-      <c r="AP49" s="17"/>
-      <c r="AR49" s="2"/>
-      <c r="AS49" s="12"/>
-      <c r="AT49" s="12"/>
-      <c r="AU49" s="12"/>
-      <c r="AV49" s="18"/>
-      <c r="AW49" s="18"/>
-      <c r="AX49" s="18"/>
+      <c r="A49" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="C49" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>211</v>
+      </c>
+      <c r="E49" t="s">
+        <v>188</v>
+      </c>
+      <c r="F49">
+        <v>1000</v>
+      </c>
+      <c r="G49">
+        <v>500</v>
+      </c>
+      <c r="H49" t="s">
+        <v>109</v>
+      </c>
+      <c r="I49" t="s">
+        <v>109</v>
+      </c>
+      <c r="J49" t="s">
+        <v>208</v>
+      </c>
+      <c r="K49" t="s">
+        <v>167</v>
+      </c>
+      <c r="L49" t="s">
+        <v>215</v>
+      </c>
+      <c r="M49" t="s">
+        <v>202</v>
+      </c>
+      <c r="N49" s="26">
+        <v>0</v>
+      </c>
+      <c r="O49" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P49" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q49">
+        <v>3</v>
+      </c>
+      <c r="R49">
+        <v>75</v>
+      </c>
+      <c r="S49">
+        <v>50</v>
+      </c>
+      <c r="T49">
+        <v>60</v>
+      </c>
+      <c r="U49" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>10</v>
+      </c>
+      <c r="X49" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y49" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z49" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA49" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB49" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC49" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD49" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE49" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF49" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG49" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH49" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI49">
+        <v>30</v>
+      </c>
+      <c r="AJ49" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK49">
+        <v>10</v>
+      </c>
+      <c r="AL49">
+        <v>200</v>
+      </c>
+      <c r="AM49" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN49">
+        <v>1</v>
+      </c>
+      <c r="AO49" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP49" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ49">
+        <v>200</v>
+      </c>
+      <c r="AR49" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS49" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT49" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU49" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV49" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW49" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX49" s="18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B50" s="31" t="s">
-        <v>284</v>
-      </c>
-      <c r="C50" s="11"/>
-      <c r="N50" s="26"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="26"/>
-      <c r="U50" s="26"/>
-      <c r="X50" s="26"/>
-      <c r="Y50" s="26"/>
-      <c r="Z50" s="26"/>
-      <c r="AA50" s="26"/>
-      <c r="AB50" s="26"/>
-      <c r="AC50" s="26"/>
-      <c r="AD50" s="41"/>
-      <c r="AE50" s="26"/>
-      <c r="AG50" s="2"/>
-      <c r="AH50" s="2"/>
-      <c r="AM50" s="2"/>
-      <c r="AO50" s="2"/>
-      <c r="AP50" s="17"/>
-      <c r="AR50" s="2"/>
-      <c r="AS50" s="12"/>
-      <c r="AT50" s="12"/>
-      <c r="AU50" s="12"/>
-      <c r="AV50" s="18"/>
-      <c r="AW50" s="18"/>
-      <c r="AX50" s="18"/>
+      <c r="A50" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="C50" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" t="s">
+        <v>211</v>
+      </c>
+      <c r="E50" t="s">
+        <v>188</v>
+      </c>
+      <c r="F50">
+        <v>1000</v>
+      </c>
+      <c r="G50">
+        <v>500</v>
+      </c>
+      <c r="H50" t="s">
+        <v>109</v>
+      </c>
+      <c r="I50" t="s">
+        <v>109</v>
+      </c>
+      <c r="J50" t="s">
+        <v>208</v>
+      </c>
+      <c r="K50" t="s">
+        <v>167</v>
+      </c>
+      <c r="L50" t="s">
+        <v>215</v>
+      </c>
+      <c r="M50" t="s">
+        <v>202</v>
+      </c>
+      <c r="N50" s="26">
+        <v>0</v>
+      </c>
+      <c r="O50" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P50" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q50">
+        <v>3</v>
+      </c>
+      <c r="R50">
+        <v>75</v>
+      </c>
+      <c r="S50">
+        <v>50</v>
+      </c>
+      <c r="T50">
+        <v>60</v>
+      </c>
+      <c r="U50" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V50">
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <v>10</v>
+      </c>
+      <c r="X50" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y50" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z50" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA50" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB50" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC50" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="AD50" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE50" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF50" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG50" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH50" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI50">
+        <v>30</v>
+      </c>
+      <c r="AJ50" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK50">
+        <v>5</v>
+      </c>
+      <c r="AL50">
+        <v>200</v>
+      </c>
+      <c r="AM50" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN50">
+        <v>1</v>
+      </c>
+      <c r="AO50" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP50" s="17">
+        <v>1</v>
+      </c>
+      <c r="AQ50">
+        <v>200</v>
+      </c>
+      <c r="AR50" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS50" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT50" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU50" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV50" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW50" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX50" s="18" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A51" s="34" t="s">
-        <v>285</v>
-      </c>
-      <c r="B51" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="C51" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
-        <v>211</v>
-      </c>
-      <c r="E51" t="s">
-        <v>188</v>
-      </c>
-      <c r="F51">
-        <v>1000</v>
-      </c>
-      <c r="G51">
-        <v>500</v>
-      </c>
-      <c r="H51" t="s">
-        <v>109</v>
-      </c>
-      <c r="I51" t="s">
-        <v>109</v>
-      </c>
-      <c r="J51" t="s">
-        <v>208</v>
-      </c>
-      <c r="K51" t="s">
-        <v>167</v>
-      </c>
-      <c r="L51" t="s">
-        <v>215</v>
-      </c>
-      <c r="M51" t="s">
-        <v>202</v>
-      </c>
-      <c r="N51" s="26">
-        <v>0</v>
-      </c>
-      <c r="O51" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P51" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q51">
-        <v>3</v>
-      </c>
-      <c r="R51">
-        <v>75</v>
-      </c>
-      <c r="S51">
-        <v>50</v>
-      </c>
-      <c r="T51">
-        <v>60</v>
-      </c>
-      <c r="U51" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V51">
-        <v>0</v>
-      </c>
-      <c r="W51">
-        <v>10</v>
-      </c>
-      <c r="X51" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y51" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z51" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA51" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB51" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC51" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD51" s="41">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AE51" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF51" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG51" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH51" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI51">
-        <v>30</v>
-      </c>
-      <c r="AJ51" t="s">
-        <v>115</v>
-      </c>
-      <c r="AK51">
-        <v>5</v>
-      </c>
-      <c r="AL51">
-        <v>200</v>
-      </c>
-      <c r="AM51" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN51">
-        <v>1</v>
-      </c>
-      <c r="AO51" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP51" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ51">
-        <v>200</v>
-      </c>
-      <c r="AR51" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS51" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT51" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU51" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV51" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW51" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX51" s="18" t="b">
-        <v>0</v>
-      </c>
+      <c r="A51" s="40"/>
+      <c r="C51" s="11"/>
+      <c r="N51" s="26"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="26"/>
+      <c r="U51" s="26"/>
+      <c r="X51" s="26"/>
+      <c r="Y51" s="26"/>
+      <c r="Z51" s="26"/>
+      <c r="AA51" s="26"/>
+      <c r="AB51" s="26"/>
+      <c r="AC51" s="26"/>
+      <c r="AD51" s="41"/>
+      <c r="AE51" s="26"/>
+      <c r="AG51" s="2"/>
+      <c r="AH51" s="2"/>
+      <c r="AM51" s="2"/>
+      <c r="AO51" s="2"/>
+      <c r="AP51" s="17"/>
+      <c r="AR51" s="2"/>
+      <c r="AS51" s="12"/>
+      <c r="AT51" s="12"/>
+      <c r="AU51" s="12"/>
+      <c r="AV51" s="18"/>
+      <c r="AW51" s="18"/>
+      <c r="AX51" s="18"/>
     </row>
     <row r="52" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A52" s="34" t="s">
+      <c r="B52" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="26"/>
+      <c r="U52" s="26"/>
+      <c r="X52" s="26"/>
+      <c r="Y52" s="26"/>
+      <c r="Z52" s="26"/>
+      <c r="AA52" s="26"/>
+      <c r="AB52" s="26"/>
+      <c r="AC52" s="26"/>
+      <c r="AD52" s="41"/>
+      <c r="AE52" s="26"/>
+      <c r="AG52" s="2"/>
+      <c r="AH52" s="2"/>
+      <c r="AM52" s="2"/>
+      <c r="AO52" s="2"/>
+      <c r="AP52" s="17"/>
+      <c r="AR52" s="2"/>
+      <c r="AS52" s="12"/>
+      <c r="AT52" s="12"/>
+      <c r="AU52" s="12"/>
+      <c r="AV52" s="18"/>
+      <c r="AW52" s="18"/>
+      <c r="AX52" s="18"/>
+    </row>
+    <row r="53" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="C53" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" t="s">
+        <v>211</v>
+      </c>
+      <c r="E53" t="s">
+        <v>188</v>
+      </c>
+      <c r="F53">
+        <v>1000</v>
+      </c>
+      <c r="G53">
+        <v>500</v>
+      </c>
+      <c r="H53" t="s">
+        <v>109</v>
+      </c>
+      <c r="I53" t="s">
+        <v>109</v>
+      </c>
+      <c r="J53" t="s">
+        <v>208</v>
+      </c>
+      <c r="K53" t="s">
+        <v>167</v>
+      </c>
+      <c r="L53" t="s">
+        <v>215</v>
+      </c>
+      <c r="M53" t="s">
+        <v>202</v>
+      </c>
+      <c r="N53" s="26">
+        <v>0</v>
+      </c>
+      <c r="O53" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P53" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q53">
+        <v>3</v>
+      </c>
+      <c r="R53">
+        <v>75</v>
+      </c>
+      <c r="S53">
+        <v>50</v>
+      </c>
+      <c r="T53">
+        <v>60</v>
+      </c>
+      <c r="U53" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53">
+        <v>10</v>
+      </c>
+      <c r="X53" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y53" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z53" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA53" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB53" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC53" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD53" s="41">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AE53" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF53" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG53" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH53" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI53">
+        <v>30</v>
+      </c>
+      <c r="AJ53" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK53">
+        <v>5</v>
+      </c>
+      <c r="AL53">
+        <v>200</v>
+      </c>
+      <c r="AM53" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN53">
+        <v>1</v>
+      </c>
+      <c r="AO53" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP53" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ53">
+        <v>200</v>
+      </c>
+      <c r="AR53" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS53" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT53" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU53" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV53" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="AW53" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX53" s="18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A54" s="34" t="s">
         <v>288</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B54" s="19" t="s">
         <v>289</v>
       </c>
-      <c r="C52" s="11" t="b">
+      <c r="C54" s="11" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" t="s">
+        <v>211</v>
+      </c>
+      <c r="E54" t="s">
+        <v>188</v>
+      </c>
+      <c r="F54">
+        <v>1000</v>
+      </c>
+      <c r="G54">
+        <v>500</v>
+      </c>
+      <c r="H54" t="s">
+        <v>109</v>
+      </c>
+      <c r="I54" t="s">
+        <v>109</v>
+      </c>
+      <c r="J54" t="s">
+        <v>208</v>
+      </c>
+      <c r="K54" t="s">
+        <v>167</v>
+      </c>
+      <c r="L54" t="s">
+        <v>215</v>
+      </c>
+      <c r="M54" t="s">
+        <v>202</v>
+      </c>
+      <c r="N54" s="26">
+        <v>0</v>
+      </c>
+      <c r="O54" s="18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P54" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="Q54">
+        <v>3</v>
+      </c>
+      <c r="R54">
+        <v>75</v>
+      </c>
+      <c r="S54">
+        <v>50</v>
+      </c>
+      <c r="T54">
+        <v>60</v>
+      </c>
+      <c r="U54" s="26">
+        <v>0.02</v>
+      </c>
+      <c r="V54">
+        <v>0</v>
+      </c>
+      <c r="W54">
+        <v>10</v>
+      </c>
+      <c r="X54" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Y54" s="26">
+        <v>0.04</v>
+      </c>
+      <c r="Z54" s="26">
+        <v>0.03</v>
+      </c>
+      <c r="AA54" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="AB54" s="26">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AC54" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD54" s="41">
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="AE54" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="AF54" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG54" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH54" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="AI54">
+        <v>30</v>
+      </c>
+      <c r="AJ54" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK54">
+        <v>5</v>
+      </c>
+      <c r="AL54">
+        <v>200</v>
+      </c>
+      <c r="AM54" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AN54">
         <v>1</v>
       </c>
-      <c r="D52" t="s">
-        <v>211</v>
-      </c>
-      <c r="E52" t="s">
-        <v>188</v>
-      </c>
-      <c r="F52">
-        <v>1000</v>
-      </c>
-      <c r="G52">
-        <v>500</v>
-      </c>
-      <c r="H52" t="s">
-        <v>109</v>
-      </c>
-      <c r="I52" t="s">
-        <v>109</v>
-      </c>
-      <c r="J52" t="s">
-        <v>208</v>
-      </c>
-      <c r="K52" t="s">
-        <v>167</v>
-      </c>
-      <c r="L52" t="s">
-        <v>215</v>
-      </c>
-      <c r="M52" t="s">
-        <v>202</v>
-      </c>
-      <c r="N52" s="26">
+      <c r="AO54" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AP54" s="17">
+        <v>0.75</v>
+      </c>
+      <c r="AQ54">
+        <v>200</v>
+      </c>
+      <c r="AR54" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AS54" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="AT54" s="12">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="AU54" s="12">
+        <v>0.05</v>
+      </c>
+      <c r="AV54" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="O52" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="P52" s="26">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="Q52">
-        <v>3</v>
-      </c>
-      <c r="R52">
-        <v>75</v>
-      </c>
-      <c r="S52">
-        <v>50</v>
-      </c>
-      <c r="T52">
-        <v>60</v>
-      </c>
-      <c r="U52" s="26">
-        <v>0.02</v>
-      </c>
-      <c r="V52">
-        <v>0</v>
-      </c>
-      <c r="W52">
-        <v>10</v>
-      </c>
-      <c r="X52" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Y52" s="26">
-        <v>0.04</v>
-      </c>
-      <c r="Z52" s="26">
-        <v>0.03</v>
-      </c>
-      <c r="AA52" s="26">
-        <v>0.01</v>
-      </c>
-      <c r="AB52" s="26">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="AC52" s="26" t="s">
-        <v>156</v>
-      </c>
-      <c r="AD52" s="41">
-        <v>8.2199999999999995E-2</v>
-      </c>
-      <c r="AE52" s="26">
-        <v>0.12</v>
-      </c>
-      <c r="AF52" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG52" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AH52" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="AI52">
-        <v>30</v>
-      </c>
-      <c r="AJ52" t="s">
-        <v>115</v>
-      </c>
-      <c r="AK52">
-        <v>5</v>
-      </c>
-      <c r="AL52">
-        <v>200</v>
-      </c>
-      <c r="AM52" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="AN52">
+      <c r="AW54" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="AO52" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AP52" s="17">
-        <v>0.75</v>
-      </c>
-      <c r="AQ52">
-        <v>200</v>
-      </c>
-      <c r="AR52" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS52" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="AT52" s="12">
-        <v>0.14499999999999999</v>
-      </c>
-      <c r="AU52" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="AV52" s="18" t="b">
-        <v>0</v>
-      </c>
-      <c r="AW52" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX52" s="18" t="b">
+      <c r="AX54" s="18" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="H4:J4"/>
     <mergeCell ref="AO4:AQ4"/>
     <mergeCell ref="P4:W4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="AG4:AI4"/>
     <mergeCell ref="AR4:AU4"/>
     <mergeCell ref="AC4:AE4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <dataValidations count="21">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM9 AM13:AM52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM6:AM9 AM13:AM54">
       <formula1>"MA,EAA"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH9 AH13:AH52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH6:AH9 AH13:AH54">
       <formula1>"cd,cp,sl"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AG9 AG13:AG52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG6:AG9 AG13:AG54">
       <formula1>"open,closed"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR6:AR9 AR13:AR52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR6:AR9 AR13:AR54">
       <formula1>ConPolicy</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O9 C6:C10 O13:O52 C13:C52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O9 C6:C10 C13:C54 O13:O54">
       <formula1>"TRUE,FALSE"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="AA6:AA9 U6:U9 AA13:AA52 U13:U52">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-10% please" sqref="AA6:AA9 U6:U9 AA13:AA54 U13:U54">
       <formula1>0</formula1>
       <formula2>0.1</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="V6:W9 V13:W52">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0-15" sqref="V6:W9 V13:W54">
       <formula1>0</formula1>
       <formula2>15</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Z9 AB6:AB9 AD6:AD9 X13:Z52 AB13:AB52 AD13:AD52">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="X6:Z9 AB6:AB9 AD6:AD9 X13:Z54 AB13:AB54 AD13:AD54">
       <formula1>0</formula1>
       <formula2>0.2</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AI6:AI9 AI13:AI52">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 0 to 30, please" sqref="AI6:AI9 AI13:AI54">
       <formula1>0</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AS6:AT9 AS13:AT52">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75%" sqref="AS6:AT9 AS13:AT54">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AU6:AU9 AU13:AU52">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-30%" sqref="AU6:AU9 AU13:AU54">
       <formula1>0</formula1>
       <formula2>0.3</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AE6:AE9 AE13:AE52">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-75% please" sqref="AE6:AE9 AE13:AE54">
       <formula1>0</formula1>
       <formula2>0.75</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AK6:AK9 AK13:AK52">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer, 1 to 30" sqref="AK6:AK9 AK13:AK54">
       <formula1>1</formula1>
       <formula2>30</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL9 AL13:AL52">
+    <dataValidation type="decimal" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL6:AL9 AL13:AL54">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN13:AN52">
+    <dataValidation type="decimal" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN13:AN54">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AC6:AC9 AC13:AC52"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV6:AX9 AV13:AX52">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Decimal, 0-20% please" sqref="AC6:AC9 AC13:AC54"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV6:AX9 AV13:AX54">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO9 AO13:AO52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO6:AO9 AO13:AO54">
       <formula1>"MA,AL,AL_pct"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP9 AP13:AP52">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP6:AP9 AP13:AP54">
       <formula1>0</formula1>
       <formula2>1.5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="R6:R9 R13:R52">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Integer 55 to 65, please" sqref="R6:R9 R13:R54">
       <formula1>35</formula1>
       <formula2>80</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:I9 H13:I52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:I9 H13:I54">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -8293,37 +8608,37 @@
           <x14:formula1>
             <xm:f>DropDowns!$A$57:$A$61</xm:f>
           </x14:formula1>
-          <xm:sqref>K6:K9 K13:K52</xm:sqref>
+          <xm:sqref>K6:K9 K13:K54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$64:$A$71</xm:f>
           </x14:formula1>
-          <xm:sqref>L6:L9 L13:L52</xm:sqref>
+          <xm:sqref>L6:L9 L13:L54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$45:$A$52</xm:f>
           </x14:formula1>
-          <xm:sqref>E6:E9 E13:E52</xm:sqref>
+          <xm:sqref>E6:E9 E13:E54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$29:$A$42</xm:f>
           </x14:formula1>
-          <xm:sqref>D6:D9 D13:D52</xm:sqref>
+          <xm:sqref>D6:D9 D13:D54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$21:$A$24</xm:f>
           </x14:formula1>
-          <xm:sqref>J6:J9 J13:J52</xm:sqref>
+          <xm:sqref>J6:J9 J13:J54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DropDowns!$A$74:$A$77</xm:f>
           </x14:formula1>
-          <xm:sqref>M6:M9 M13:M52</xm:sqref>
+          <xm:sqref>M6:M9 M13:M54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
update for M1 report
</commit_message>
<xml_diff>
--- a/IO_M1_new/RunControl_M1_new.xlsx
+++ b/IO_M1_new/RunControl_M1_new.xlsx
@@ -1402,10 +1402,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1414,13 +1411,16 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2104,7 +2104,7 @@
   <dimension ref="A1:AY54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="T18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="X42" sqref="X42"/>
@@ -2302,62 +2302,62 @@
       </c>
     </row>
     <row r="4" spans="1:51" s="8" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="46"/>
       <c r="D4" s="42"/>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="44"/>
+      <c r="F4" s="48"/>
       <c r="G4" s="27"/>
       <c r="H4" s="27"/>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="45" t="s">
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="45"/>
+      <c r="M4" s="44"/>
       <c r="N4" s="28"/>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="P4" s="46"/>
-      <c r="Q4" s="45" t="s">
+      <c r="P4" s="45"/>
+      <c r="Q4" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
+      <c r="R4" s="44"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="44"/>
+      <c r="U4" s="44"/>
+      <c r="V4" s="44"/>
+      <c r="W4" s="44"/>
+      <c r="X4" s="44"/>
       <c r="Y4" s="29"/>
       <c r="Z4" s="29"/>
-      <c r="AA4" s="46" t="s">
+      <c r="AA4" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AB4" s="46"/>
-      <c r="AC4" s="46"/>
-      <c r="AD4" s="48" t="s">
+      <c r="AB4" s="45"/>
+      <c r="AC4" s="45"/>
+      <c r="AD4" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="AE4" s="48"/>
-      <c r="AF4" s="48"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="43"/>
       <c r="AG4" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AH4" s="43" t="s">
+      <c r="AH4" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="AI4" s="43"/>
-      <c r="AJ4" s="43"/>
+      <c r="AI4" s="46"/>
+      <c r="AJ4" s="46"/>
       <c r="AK4" s="21" t="s">
         <v>70</v>
       </c>
@@ -2365,17 +2365,17 @@
       <c r="AM4" s="21"/>
       <c r="AN4" s="21"/>
       <c r="AO4" s="21"/>
-      <c r="AP4" s="48" t="s">
+      <c r="AP4" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="AQ4" s="48"/>
-      <c r="AR4" s="48"/>
-      <c r="AS4" s="49" t="s">
+      <c r="AQ4" s="43"/>
+      <c r="AR4" s="43"/>
+      <c r="AS4" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="AT4" s="49"/>
-      <c r="AU4" s="49"/>
-      <c r="AV4" s="49"/>
+      <c r="AT4" s="47"/>
+      <c r="AU4" s="47"/>
+      <c r="AV4" s="47"/>
       <c r="AW4" s="15"/>
       <c r="AX4" s="22"/>
       <c r="AY4" s="20"/>
@@ -8676,17 +8676,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="I4:K4"/>
     <mergeCell ref="AP4:AR4"/>
     <mergeCell ref="Q4:X4"/>
     <mergeCell ref="AA4:AC4"/>
     <mergeCell ref="AH4:AJ4"/>
     <mergeCell ref="AS4:AV4"/>
     <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="I4:K4"/>
   </mergeCells>
   <dataValidations count="21">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN6:AN9 AN13:AN54">

</xml_diff>

<commit_message>
update for riskSharing inputs
</commit_message>
<xml_diff>
--- a/IO_M1_new/RunControl_M1_new.xlsx
+++ b/IO_M1_new/RunControl_M1_new.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\PenSim-Projects\Model_Main\IO_M1_new\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9AB532-8D27-42A7-8C11-E11FBBE729ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E0B5AC-3A4F-49E7-BE0D-14386C3B0FB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
     <sheet name="RunControl" sheetId="3" r:id="rId3"/>
-    <sheet name="Returns" sheetId="6" r:id="rId4"/>
-    <sheet name="Contributions" sheetId="7" r:id="rId5"/>
-    <sheet name="GlobalParams" sheetId="4" r:id="rId6"/>
+    <sheet name="GlobalParams" sheetId="4" r:id="rId4"/>
+    <sheet name="Returns" sheetId="6" r:id="rId5"/>
+    <sheet name="Contributions" sheetId="7" r:id="rId6"/>
     <sheet name="DropDowns" sheetId="5" r:id="rId7"/>
     <sheet name="RunList_M1" sheetId="10" r:id="rId8"/>
     <sheet name="RunList_M2.1" sheetId="11" r:id="rId9"/>
@@ -28,7 +28,7 @@
     <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Returns!$A$3:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Returns!$A$3:$D$6</definedName>
     <definedName name="ConPolicy">DropDowns!$A$12:$A$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -36,7 +36,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2120,11 +2122,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="N9" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="5" topLeftCell="K9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="Q16" sqref="Q16"/>
+      <selection pane="bottomRight" activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8837,6 +8839,76 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1025" width="8.5703125"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>81</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:D13"/>
   <sheetViews>
@@ -9018,7 +9090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:D5"/>
   <sheetViews>
@@ -9059,76 +9131,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1025" width="8.5703125"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>100</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>20</v>
-      </c>
-      <c r="G3">
-        <v>75</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 

</xml_diff>